<commit_message>
Se actualiza el documento APPMO-SP_ARP_v1.1.xlsx
</commit_message>
<xml_diff>
--- a/Entregables/V. Análisis de riesgo del proyecto de TI/APPMO-SP_ARP_v1.1.xlsx
+++ b/Entregables/V. Análisis de riesgo del proyecto de TI/APPMO-SP_ARP_v1.1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FRANC\Desktop\SM-ROOT\Entregables\V. Análisis de riesgo del proyecto de TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
   <si>
     <t>•Realizar pruebas completas sobre cada módulo de la aplicación asegurandose de cumplir la funcionalidad principal
 •Darle seguimiento a cada falla encontrado
-•someter nuevs mente a pruebas los módulos donde se reportaron fallas</t>
+•someter nuevamente a pruebas los módulos donde se reportaron fallas</t>
   </si>
 </sst>
 </file>
@@ -1548,6 +1548,54 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1575,6 +1623,51 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1584,49 +1677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1635,9 +1686,6 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1646,54 +1694,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2045,41 +2045,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:G21"/>
+    <sheetView topLeftCell="B14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
-    <col min="12" max="1023" width="8.5703125" customWidth="1"/>
+    <col min="12" max="1023" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="118" t="s">
+    <row r="1" spans="2:11" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="120"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="136"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="26"/>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2091,7 +2091,7 @@
       <c r="J2" s="27"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2103,23 +2103,23 @@
       <c r="J3" s="13"/>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="125" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="141"/>
+      <c r="D4" s="141"/>
       <c r="E4" s="13"/>
-      <c r="F4" s="125" t="s">
+      <c r="F4" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="125"/>
-      <c r="H4" s="125"/>
-      <c r="I4" s="125"/>
+      <c r="G4" s="141"/>
+      <c r="H4" s="141"/>
+      <c r="I4" s="141"/>
       <c r="J4" s="13"/>
       <c r="K4" s="14"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>5</v>
       </c>
@@ -2136,14 +2136,14 @@
       <c r="G5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="121" t="s">
+      <c r="H5" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="121"/>
+      <c r="I5" s="137"/>
       <c r="J5" s="13"/>
       <c r="K5" s="14"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -2160,14 +2160,14 @@
       <c r="G6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="121" t="s">
+      <c r="H6" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="121"/>
+      <c r="I6" s="137"/>
       <c r="J6" s="13"/>
       <c r="K6" s="14"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>3</v>
       </c>
@@ -2184,14 +2184,14 @@
       <c r="G7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="121" t="s">
+      <c r="H7" s="137" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="121"/>
+      <c r="I7" s="137"/>
       <c r="J7" s="13"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>2</v>
       </c>
@@ -2208,14 +2208,14 @@
       <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="121" t="s">
+      <c r="H8" s="137" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="121"/>
+      <c r="I8" s="137"/>
       <c r="J8" s="13"/>
       <c r="K8" s="14"/>
     </row>
-    <row r="9" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>1</v>
       </c>
@@ -2232,14 +2232,14 @@
       <c r="G9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="122" t="s">
+      <c r="H9" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="122"/>
+      <c r="I9" s="138"/>
       <c r="J9" s="13"/>
       <c r="K9" s="14"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -2251,7 +2251,7 @@
       <c r="J10" s="13"/>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -2263,7 +2263,7 @@
       <c r="J11" s="13"/>
       <c r="K11" s="14"/>
     </row>
-    <row r="12" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -2275,19 +2275,19 @@
       <c r="J12" s="13"/>
       <c r="K12" s="14"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="123" t="s">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="139" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
-      <c r="H13" s="124" t="s">
+      <c r="C13" s="139"/>
+      <c r="D13" s="139"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="139"/>
+      <c r="G13" s="139"/>
+      <c r="H13" s="140" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="124"/>
+      <c r="I13" s="140"/>
       <c r="J13" s="8" t="s">
         <v>23</v>
       </c>
@@ -2295,19 +2295,19 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="117"/>
-      <c r="C14" s="117"/>
-      <c r="D14" s="117"/>
-      <c r="E14" s="117"/>
-      <c r="F14" s="117"/>
-      <c r="G14" s="117"/>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="133"/>
+      <c r="C14" s="133"/>
+      <c r="D14" s="133"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
+      <c r="G14" s="133"/>
       <c r="H14" s="9"/>
       <c r="I14" s="10"/>
       <c r="J14" s="11"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="2:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
         <v>24</v>
       </c>
@@ -2339,23 +2339,23 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="98">
         <v>1</v>
       </c>
       <c r="C16" s="99" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="154" t="s">
+      <c r="D16" s="121" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="155" t="s">
+      <c r="E16" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="F16" s="156" t="s">
+      <c r="F16" s="123" t="s">
         <v>111</v>
       </c>
-      <c r="G16" s="157" t="s">
+      <c r="G16" s="124" t="s">
         <v>112</v>
       </c>
       <c r="H16" s="109">
@@ -2368,27 +2368,27 @@
         <f t="shared" ref="J16:J30" si="0">H16*I16</f>
         <v>12</v>
       </c>
-      <c r="K16" s="150" t="s">
+      <c r="K16" s="117" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="20">
         <v>2</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="158" t="s">
+      <c r="D17" s="125" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="159" t="s">
+      <c r="E17" s="126" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="160" t="s">
+      <c r="F17" s="127" t="s">
         <v>114</v>
       </c>
-      <c r="G17" s="161" t="s">
+      <c r="G17" s="128" t="s">
         <v>115</v>
       </c>
       <c r="H17" s="111">
@@ -2401,27 +2401,27 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="K17" s="151" t="s">
+      <c r="K17" s="118" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="22">
         <v>3</v>
       </c>
       <c r="C18" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="162" t="s">
+      <c r="D18" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="163" t="s">
+      <c r="E18" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="164" t="s">
+      <c r="F18" s="131" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="165" t="s">
+      <c r="G18" s="132" t="s">
         <v>93</v>
       </c>
       <c r="H18" s="113">
@@ -2434,27 +2434,27 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="K18" s="152" t="s">
+      <c r="K18" s="119" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" ht="70.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="22">
         <v>4</v>
       </c>
       <c r="C19" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="162" t="s">
+      <c r="D19" s="129" t="s">
         <v>105</v>
       </c>
-      <c r="E19" s="163" t="s">
+      <c r="E19" s="130" t="s">
         <v>118</v>
       </c>
-      <c r="F19" s="164" t="s">
+      <c r="F19" s="131" t="s">
         <v>120</v>
       </c>
-      <c r="G19" s="165" t="s">
+      <c r="G19" s="132" t="s">
         <v>119</v>
       </c>
       <c r="H19" s="113">
@@ -2467,27 +2467,27 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K19" s="153" t="s">
+      <c r="K19" s="120" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="22">
         <v>5</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="162" t="s">
+      <c r="D20" s="129" t="s">
         <v>122</v>
       </c>
-      <c r="E20" s="163" t="s">
+      <c r="E20" s="130" t="s">
         <v>123</v>
       </c>
-      <c r="F20" s="164" t="s">
+      <c r="F20" s="131" t="s">
         <v>125</v>
       </c>
-      <c r="G20" s="165" t="s">
+      <c r="G20" s="132" t="s">
         <v>124</v>
       </c>
       <c r="H20" s="113">
@@ -2500,27 +2500,27 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="K20" s="153" t="s">
+      <c r="K20" s="120" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="22">
         <v>6</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="162" t="s">
+      <c r="D21" s="129" t="s">
         <v>97</v>
       </c>
-      <c r="E21" s="163" t="s">
+      <c r="E21" s="130" t="s">
         <v>98</v>
       </c>
-      <c r="F21" s="164" t="s">
+      <c r="F21" s="131" t="s">
         <v>106</v>
       </c>
-      <c r="G21" s="165" t="s">
+      <c r="G21" s="132" t="s">
         <v>96</v>
       </c>
       <c r="H21" s="113">
@@ -2533,11 +2533,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="K21" s="152" t="s">
+      <c r="K21" s="119" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="22">
         <v>7</v>
       </c>
@@ -2558,7 +2558,7 @@
       </c>
       <c r="K22" s="100"/>
     </row>
-    <row r="23" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="22">
         <v>8</v>
       </c>
@@ -2579,7 +2579,7 @@
       </c>
       <c r="K23" s="100"/>
     </row>
-    <row r="24" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="22">
         <v>9</v>
       </c>
@@ -2600,7 +2600,7 @@
       </c>
       <c r="K24" s="100"/>
     </row>
-    <row r="25" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="22">
         <v>10</v>
       </c>
@@ -2621,7 +2621,7 @@
       </c>
       <c r="K25" s="100"/>
     </row>
-    <row r="26" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="22">
         <v>11</v>
       </c>
@@ -2642,7 +2642,7 @@
       </c>
       <c r="K26" s="100"/>
     </row>
-    <row r="27" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="22">
         <v>12</v>
       </c>
@@ -2663,7 +2663,7 @@
       </c>
       <c r="K27" s="100"/>
     </row>
-    <row r="28" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="22">
         <v>13</v>
       </c>
@@ -2684,7 +2684,7 @@
       </c>
       <c r="K28" s="100"/>
     </row>
-    <row r="29" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="22">
         <v>14</v>
       </c>
@@ -2705,7 +2705,7 @@
       </c>
       <c r="K29" s="100"/>
     </row>
-    <row r="30" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="24">
         <v>15</v>
       </c>
@@ -2726,7 +2726,7 @@
       </c>
       <c r="K30" s="101"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -2738,7 +2738,7 @@
       <c r="J31" s="13"/>
       <c r="K31" s="14"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="12"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -2750,7 +2750,7 @@
       <c r="J32" s="13"/>
       <c r="K32" s="14"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -2762,7 +2762,7 @@
       <c r="J33" s="13"/>
       <c r="K33" s="14"/>
     </row>
-    <row r="34" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="75"/>
       <c r="C34" s="76"/>
       <c r="D34" s="76"/>
@@ -2801,24 +2801,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q50"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="26"/>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2832,23 +2832,23 @@
       <c r="L2" s="27"/>
       <c r="M2" s="28"/>
     </row>
-    <row r="3" spans="2:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
-      <c r="C3" s="126" t="s">
+      <c r="C3" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="126"/>
-      <c r="J3" s="126"/>
-      <c r="K3" s="126"/>
-      <c r="L3" s="126"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="157"/>
+      <c r="H3" s="157"/>
+      <c r="I3" s="157"/>
+      <c r="J3" s="157"/>
+      <c r="K3" s="157"/>
+      <c r="L3" s="157"/>
       <c r="M3" s="14"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -2862,7 +2862,7 @@
       <c r="L4" s="13"/>
       <c r="M4" s="14"/>
     </row>
-    <row r="5" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="12"/>
       <c r="C5" s="29" t="s">
         <v>0</v>
@@ -2881,16 +2881,16 @@
       <c r="I5" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="127" t="s">
+      <c r="J5" s="158" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="127"/>
+      <c r="K5" s="158"/>
       <c r="L5" s="34" t="s">
         <v>36</v>
       </c>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B6" s="12"/>
       <c r="C6" s="35" t="s">
         <v>37</v>
@@ -2909,17 +2909,17 @@
       <c r="I6" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="128" t="s">
+      <c r="J6" s="159" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="128"/>
+      <c r="K6" s="159"/>
       <c r="L6" s="37">
         <f>16/25*100</f>
         <v>64</v>
       </c>
       <c r="M6" s="14"/>
     </row>
-    <row r="7" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="C7" s="40" t="s">
         <v>41</v>
@@ -2938,17 +2938,17 @@
       <c r="I7" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="129" t="s">
+      <c r="J7" s="153" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="129"/>
+      <c r="K7" s="153"/>
       <c r="L7" s="42">
         <f>15/25*100</f>
         <v>60</v>
       </c>
       <c r="M7" s="14"/>
     </row>
-    <row r="8" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
       <c r="C8" s="40" t="s">
         <v>45</v>
@@ -2967,17 +2967,17 @@
       <c r="I8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="129" t="s">
+      <c r="J8" s="153" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="129"/>
+      <c r="K8" s="153"/>
       <c r="L8" s="42">
         <f>12/25*100</f>
         <v>48</v>
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" s="40" t="s">
         <v>47</v>
@@ -2996,17 +2996,17 @@
       <c r="I9" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="129" t="s">
+      <c r="J9" s="153" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="129"/>
+      <c r="K9" s="153"/>
       <c r="L9" s="42">
         <f>8/25*100</f>
         <v>32</v>
       </c>
       <c r="M9" s="14"/>
     </row>
-    <row r="10" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
       <c r="C10" s="45" t="s">
         <v>49</v>
@@ -3025,10 +3025,10 @@
       <c r="I10" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="130" t="s">
+      <c r="J10" s="154" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="130"/>
+      <c r="K10" s="154"/>
       <c r="L10" s="47">
         <f>5/25*100</f>
         <v>20</v>
@@ -3039,7 +3039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="12"/>
       <c r="C11" s="49"/>
       <c r="D11" s="13"/>
@@ -3053,7 +3053,7 @@
       <c r="L11" s="13"/>
       <c r="M11" s="14"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -3067,17 +3067,17 @@
       <c r="L12" s="13"/>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="2:17" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="131" t="s">
+      <c r="D13" s="155" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="131"/>
+      <c r="E13" s="155"/>
       <c r="F13" s="51" t="s">
         <v>54</v>
       </c>
@@ -3101,17 +3101,17 @@
       </c>
       <c r="M13" s="14"/>
     </row>
-    <row r="14" spans="2:17" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" ht="88.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="53" t="str">
         <f>CONCATENATE($B$13,Matriz!B16)</f>
         <v>R1</v>
       </c>
-      <c r="D14" s="132" t="str">
+      <c r="D14" s="156" t="str">
         <f>Matriz!E16</f>
         <v>no trabajar eficientemente</v>
       </c>
-      <c r="E14" s="132"/>
+      <c r="E14" s="156"/>
       <c r="F14" s="54" t="str">
         <f>Matriz!F16</f>
         <v xml:space="preserve">Mala comunicación, descuerdos en el equipo y trabajo disperso. </v>
@@ -3139,17 +3139,17 @@
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="2:17" ht="61.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17" ht="79.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B17)</f>
         <v>R2</v>
       </c>
-      <c r="D15" s="133" t="str">
+      <c r="D15" s="149" t="str">
         <f>Matriz!E17</f>
         <v>Tiempos incongruentes y fechas mal planeadas ,Organización ineficiente</v>
       </c>
-      <c r="E15" s="133"/>
+      <c r="E15" s="149"/>
       <c r="F15" s="58" t="str">
         <f>Matriz!F17</f>
         <v xml:space="preserve"> Retrazo en entregables del proyecto e información dispersa</v>
@@ -3179,17 +3179,17 @@
       </c>
       <c r="M15" s="14"/>
     </row>
-    <row r="16" spans="2:17" ht="55.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="12"/>
       <c r="C16" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B18)</f>
         <v>R3</v>
       </c>
-      <c r="D16" s="133" t="str">
+      <c r="D16" s="149" t="str">
         <f>Matriz!E18</f>
         <v>Cambios regulares y nuevos añadidos a los requerimientos</v>
       </c>
-      <c r="E16" s="133"/>
+      <c r="E16" s="149"/>
       <c r="F16" s="107" t="str">
         <f>Matriz!F18</f>
         <v>Requerimientos ambiguos o incompletos</v>
@@ -3219,17 +3219,17 @@
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:13" ht="86.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" ht="86.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="C17" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B19)</f>
         <v>R4</v>
       </c>
-      <c r="D17" s="133" t="str">
+      <c r="D17" s="149" t="str">
         <f>Matriz!E19</f>
         <v>interpretación erronea de las ventanas e interfaces</v>
       </c>
-      <c r="E17" s="133"/>
+      <c r="E17" s="149"/>
       <c r="F17" s="107" t="str">
         <f>Matriz!F19</f>
         <v>Diseño de interfaces equivocadas o mal diseñadas</v>
@@ -3259,17 +3259,17 @@
       </c>
       <c r="M17" s="14"/>
     </row>
-    <row r="18" spans="2:13" ht="95.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" ht="95.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="C18" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B20)</f>
         <v>R5</v>
       </c>
-      <c r="D18" s="133" t="str">
+      <c r="D18" s="149" t="str">
         <f>Matriz!E20</f>
         <v>Estructuración erronea de los datos, tablas mal relacionadas</v>
       </c>
-      <c r="E18" s="133"/>
+      <c r="E18" s="149"/>
       <c r="F18" s="58" t="str">
         <f>Matriz!F20</f>
         <v>Retrazo en codificación del producto</v>
@@ -3299,17 +3299,17 @@
       </c>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:13" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>
       <c r="C19" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B21)</f>
         <v>R6</v>
       </c>
-      <c r="D19" s="133" t="str">
+      <c r="D19" s="149" t="str">
         <f>Matriz!E21</f>
         <v>Pruebas ineficientes</v>
       </c>
-      <c r="E19" s="133"/>
+      <c r="E19" s="149"/>
       <c r="F19" s="58" t="str">
         <f>Matriz!F21</f>
         <v>Mala ejecución del producto, presenta errores</v>
@@ -3339,17 +3339,17 @@
       </c>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="12"/>
       <c r="C20" s="53" t="str">
         <f>CONCATENATE($B$13,Matriz!B22)</f>
         <v>R7</v>
       </c>
-      <c r="D20" s="133">
+      <c r="D20" s="149">
         <f>Matriz!E22</f>
         <v>0</v>
       </c>
-      <c r="E20" s="133"/>
+      <c r="E20" s="149"/>
       <c r="F20" s="58">
         <f>Matriz!F22</f>
         <v>0</v>
@@ -3377,17 +3377,17 @@
       </c>
       <c r="M20" s="14"/>
     </row>
-    <row r="21" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="12"/>
       <c r="C21" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B23)</f>
         <v>R8</v>
       </c>
-      <c r="D21" s="133">
+      <c r="D21" s="149">
         <f>Matriz!E23</f>
         <v>0</v>
       </c>
-      <c r="E21" s="133"/>
+      <c r="E21" s="149"/>
       <c r="F21" s="58">
         <f>Matriz!F23</f>
         <v>0</v>
@@ -3415,17 +3415,17 @@
       </c>
       <c r="M21" s="14"/>
     </row>
-    <row r="22" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="C22" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B24)</f>
         <v>R9</v>
       </c>
-      <c r="D22" s="133">
+      <c r="D22" s="149">
         <f>Matriz!E24</f>
         <v>0</v>
       </c>
-      <c r="E22" s="133"/>
+      <c r="E22" s="149"/>
       <c r="F22" s="58">
         <f>Matriz!F24</f>
         <v>0</v>
@@ -3453,17 +3453,17 @@
       </c>
       <c r="M22" s="14"/>
     </row>
-    <row r="23" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="12"/>
       <c r="C23" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B25)</f>
         <v>R10</v>
       </c>
-      <c r="D23" s="133">
+      <c r="D23" s="149">
         <f>Matriz!E25</f>
         <v>0</v>
       </c>
-      <c r="E23" s="133"/>
+      <c r="E23" s="149"/>
       <c r="F23" s="58">
         <f>Matriz!F25</f>
         <v>0</v>
@@ -3491,17 +3491,17 @@
       </c>
       <c r="M23" s="14"/>
     </row>
-    <row r="24" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="12"/>
       <c r="C24" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B26)</f>
         <v>R11</v>
       </c>
-      <c r="D24" s="133">
+      <c r="D24" s="149">
         <f>Matriz!E26</f>
         <v>0</v>
       </c>
-      <c r="E24" s="133"/>
+      <c r="E24" s="149"/>
       <c r="F24" s="58">
         <f>Matriz!F26</f>
         <v>0</v>
@@ -3529,17 +3529,17 @@
       </c>
       <c r="M24" s="14"/>
     </row>
-    <row r="25" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="12"/>
       <c r="C25" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B27)</f>
         <v>R12</v>
       </c>
-      <c r="D25" s="133">
+      <c r="D25" s="149">
         <f>Matriz!E27</f>
         <v>0</v>
       </c>
-      <c r="E25" s="133"/>
+      <c r="E25" s="149"/>
       <c r="F25" s="58">
         <f>Matriz!F27</f>
         <v>0</v>
@@ -3567,17 +3567,17 @@
       </c>
       <c r="M25" s="14"/>
     </row>
-    <row r="26" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="12"/>
       <c r="C26" s="53" t="str">
         <f>CONCATENATE($B$13,Matriz!B28)</f>
         <v>R13</v>
       </c>
-      <c r="D26" s="133">
+      <c r="D26" s="149">
         <f>Matriz!E28</f>
         <v>0</v>
       </c>
-      <c r="E26" s="133"/>
+      <c r="E26" s="149"/>
       <c r="F26" s="58">
         <f>Matriz!F28</f>
         <v>0</v>
@@ -3605,17 +3605,17 @@
       </c>
       <c r="M26" s="14"/>
     </row>
-    <row r="27" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="12"/>
       <c r="C27" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B29)</f>
         <v>R14</v>
       </c>
-      <c r="D27" s="133">
+      <c r="D27" s="149">
         <f>Matriz!E29</f>
         <v>0</v>
       </c>
-      <c r="E27" s="133"/>
+      <c r="E27" s="149"/>
       <c r="F27" s="58">
         <f>Matriz!F29</f>
         <v>0</v>
@@ -3643,17 +3643,17 @@
       </c>
       <c r="M27" s="14"/>
     </row>
-    <row r="28" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="12"/>
       <c r="C28" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B30)</f>
         <v>R15</v>
       </c>
-      <c r="D28" s="133">
+      <c r="D28" s="149">
         <f>Matriz!E30</f>
         <v>0</v>
       </c>
-      <c r="E28" s="133"/>
+      <c r="E28" s="149"/>
       <c r="F28" s="58">
         <f>Matriz!F30</f>
         <v>0</v>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="M28" s="14"/>
     </row>
-    <row r="29" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -3695,23 +3695,23 @@
       <c r="L29" s="13"/>
       <c r="M29" s="14"/>
     </row>
-    <row r="30" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="134" t="s">
+    <row r="30" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="150" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="134"/>
-      <c r="D30" s="134"/>
-      <c r="E30" s="134"/>
-      <c r="F30" s="134"/>
-      <c r="G30" s="134"/>
-      <c r="H30" s="134"/>
-      <c r="I30" s="134"/>
-      <c r="J30" s="134"/>
-      <c r="K30" s="134"/>
-      <c r="L30" s="134"/>
-      <c r="M30" s="134"/>
-    </row>
-    <row r="31" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="150"/>
+      <c r="D30" s="150"/>
+      <c r="E30" s="150"/>
+      <c r="F30" s="150"/>
+      <c r="G30" s="150"/>
+      <c r="H30" s="150"/>
+      <c r="I30" s="150"/>
+      <c r="J30" s="150"/>
+      <c r="K30" s="150"/>
+      <c r="L30" s="150"/>
+      <c r="M30" s="150"/>
+    </row>
+    <row r="31" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -3725,15 +3725,15 @@
       <c r="L31" s="13"/>
       <c r="M31" s="14"/>
     </row>
-    <row r="32" spans="2:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="12"/>
       <c r="C32" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="135" t="s">
+      <c r="D32" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="E32" s="135"/>
+      <c r="E32" s="151"/>
       <c r="F32" s="63" t="s">
         <v>62</v>
       </c>
@@ -3749,23 +3749,23 @@
       <c r="J32" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="K32" s="136" t="s">
+      <c r="K32" s="152" t="s">
         <v>66</v>
       </c>
-      <c r="L32" s="136"/>
+      <c r="L32" s="152"/>
       <c r="M32" s="14"/>
     </row>
-    <row r="33" spans="2:13" ht="163.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" ht="163.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="12"/>
       <c r="C33" s="64" t="str">
         <f t="shared" ref="C33:D47" si="3">C14</f>
         <v>R1</v>
       </c>
-      <c r="D33" s="137" t="str">
+      <c r="D33" s="146" t="str">
         <f t="shared" si="3"/>
         <v>no trabajar eficientemente</v>
       </c>
-      <c r="E33" s="137"/>
+      <c r="E33" s="146"/>
       <c r="F33" s="66" t="str">
         <f t="shared" ref="F33:F47" si="4">K14</f>
         <v>MODERADO</v>
@@ -3784,25 +3784,25 @@
       <c r="J33" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="K33" s="138" t="str">
+      <c r="K33" s="147" t="str">
         <f>Matriz!K16</f>
         <v>•Realización de reuniones sobre avances del proyecto
 •Realizar acuerdos y trabajar en un punto medio de opiniones</v>
       </c>
-      <c r="L33" s="138"/>
+      <c r="L33" s="147"/>
       <c r="M33" s="14"/>
     </row>
-    <row r="34" spans="2:13" ht="53.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="12"/>
       <c r="C34" s="67" t="str">
         <f t="shared" si="3"/>
         <v>R2</v>
       </c>
-      <c r="D34" s="139" t="str">
+      <c r="D34" s="148" t="str">
         <f t="shared" si="3"/>
         <v>Tiempos incongruentes y fechas mal planeadas ,Organización ineficiente</v>
       </c>
-      <c r="E34" s="139"/>
+      <c r="E34" s="148"/>
       <c r="F34" s="68" t="str">
         <f t="shared" si="4"/>
         <v>MODERADO</v>
@@ -3820,24 +3820,24 @@
       <c r="J34" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="K34" s="140" t="str">
+      <c r="K34" s="145" t="str">
         <f>Matriz!K17</f>
         <v>Revisar actividades con fechas y ajustarlos a tiempos del proyecto, utilizar un repositorio para el almacenamiento de la información.</v>
       </c>
-      <c r="L34" s="140"/>
+      <c r="L34" s="145"/>
       <c r="M34" s="14"/>
     </row>
-    <row r="35" spans="2:13" ht="125.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" ht="125.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="12"/>
       <c r="C35" s="67" t="str">
         <f t="shared" si="3"/>
         <v>R3</v>
       </c>
-      <c r="D35" s="141" t="str">
+      <c r="D35" s="144" t="str">
         <f t="shared" si="3"/>
         <v>Cambios regulares y nuevos añadidos a los requerimientos</v>
       </c>
-      <c r="E35" s="141"/>
+      <c r="E35" s="144"/>
       <c r="F35" s="71" t="str">
         <f t="shared" si="4"/>
         <v>MODERADO</v>
@@ -3855,24 +3855,24 @@
       <c r="J35" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="K35" s="140" t="str">
+      <c r="K35" s="145" t="str">
         <f>Matriz!K18</f>
         <v xml:space="preserve">Acoplar los requerimientos nuevos cambios o existentes de forma clara y  eficiente  para cumplir la funcionalidad planeada </v>
       </c>
-      <c r="L35" s="140"/>
+      <c r="L35" s="145"/>
       <c r="M35" s="14"/>
     </row>
-    <row r="36" spans="2:13" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="12"/>
       <c r="C36" s="67" t="str">
         <f t="shared" si="3"/>
         <v>R4</v>
       </c>
-      <c r="D36" s="141" t="str">
+      <c r="D36" s="144" t="str">
         <f t="shared" si="3"/>
         <v>interpretación erronea de las ventanas e interfaces</v>
       </c>
-      <c r="E36" s="141"/>
+      <c r="E36" s="144"/>
       <c r="F36" s="68" t="str">
         <f t="shared" si="4"/>
         <v>BAJO</v>
@@ -3890,24 +3890,24 @@
       <c r="J36" s="69" t="s">
         <v>90</v>
       </c>
-      <c r="K36" s="140" t="str">
+      <c r="K36" s="145" t="str">
         <f>Matriz!K19</f>
         <v>Rediseñar las interfaces con base  a los requerimientos de software</v>
       </c>
-      <c r="L36" s="140"/>
+      <c r="L36" s="145"/>
       <c r="M36" s="14"/>
     </row>
-    <row r="37" spans="2:13" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="12"/>
       <c r="C37" s="67" t="str">
         <f t="shared" si="3"/>
         <v>R5</v>
       </c>
-      <c r="D37" s="141" t="str">
+      <c r="D37" s="144" t="str">
         <f t="shared" si="3"/>
         <v>Estructuración erronea de los datos, tablas mal relacionadas</v>
       </c>
-      <c r="E37" s="141"/>
+      <c r="E37" s="144"/>
       <c r="F37" s="71" t="str">
         <f t="shared" si="4"/>
         <v>MODERADO</v>
@@ -3925,14 +3925,14 @@
       <c r="J37" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="K37" s="140" t="str">
+      <c r="K37" s="145" t="str">
         <f>Matriz!K20</f>
         <v>Redefinir la arquitectura lógica llevando a cabo un analisis produndo para lograr  relaciones de tablas correctas con base a los procesos de la empresa</v>
       </c>
-      <c r="L37" s="140"/>
+      <c r="L37" s="145"/>
       <c r="M37" s="14"/>
     </row>
-    <row r="38" spans="2:13" ht="194.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" ht="194.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="12"/>
       <c r="C38" s="72" t="str">
         <f t="shared" si="3"/>
@@ -3954,7 +3954,7 @@
         <f>Matriz!K21</f>
         <v>•Realizar pruebas completas sobre cada módulo de la aplicación asegurandose de cumplir la funcionalidad principal
 •Darle seguimiento a cada falla encontrado
-•someter nuevs mente a pruebas los módulos donde se reportaron fallas</v>
+•someter nuevamente a pruebas los módulos donde se reportaron fallas</v>
       </c>
       <c r="I38" s="65" t="s">
         <v>67</v>
@@ -3966,12 +3966,12 @@
         <f>Matriz!K21</f>
         <v>•Realizar pruebas completas sobre cada módulo de la aplicación asegurandose de cumplir la funcionalidad principal
 •Darle seguimiento a cada falla encontrado
-•someter nuevs mente a pruebas los módulos donde se reportaron fallas</v>
+•someter nuevamente a pruebas los módulos donde se reportaron fallas</v>
       </c>
       <c r="L38" s="143"/>
       <c r="M38" s="14"/>
     </row>
-    <row r="39" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="12"/>
       <c r="C39" s="67" t="str">
         <f t="shared" si="3"/>
@@ -4002,7 +4002,7 @@
       <c r="L39" s="143"/>
       <c r="M39" s="14"/>
     </row>
-    <row r="40" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="12"/>
       <c r="C40" s="67" t="str">
         <f t="shared" si="3"/>
@@ -4033,7 +4033,7 @@
       <c r="L40" s="143"/>
       <c r="M40" s="14"/>
     </row>
-    <row r="41" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="12"/>
       <c r="C41" s="67" t="str">
         <f t="shared" si="3"/>
@@ -4064,7 +4064,7 @@
       <c r="L41" s="143"/>
       <c r="M41" s="14"/>
     </row>
-    <row r="42" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="12"/>
       <c r="C42" s="67" t="str">
         <f t="shared" si="3"/>
@@ -4095,7 +4095,7 @@
       <c r="L42" s="143"/>
       <c r="M42" s="14"/>
     </row>
-    <row r="43" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="12"/>
       <c r="C43" s="72" t="str">
         <f t="shared" si="3"/>
@@ -4126,7 +4126,7 @@
       <c r="L43" s="143"/>
       <c r="M43" s="14"/>
     </row>
-    <row r="44" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="12"/>
       <c r="C44" s="67" t="str">
         <f t="shared" si="3"/>
@@ -4157,7 +4157,7 @@
       <c r="L44" s="143"/>
       <c r="M44" s="14"/>
     </row>
-    <row r="45" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="12"/>
       <c r="C45" s="67" t="str">
         <f t="shared" si="3"/>
@@ -4188,7 +4188,7 @@
       <c r="L45" s="143"/>
       <c r="M45" s="14"/>
     </row>
-    <row r="46" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="12"/>
       <c r="C46" s="67" t="str">
         <f t="shared" si="3"/>
@@ -4219,7 +4219,7 @@
       <c r="L46" s="143"/>
       <c r="M46" s="14"/>
     </row>
-    <row r="47" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="12"/>
       <c r="C47" s="67" t="str">
         <f t="shared" si="3"/>
@@ -4250,7 +4250,7 @@
       <c r="L47" s="143"/>
       <c r="M47" s="14"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="12"/>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
@@ -4264,7 +4264,7 @@
       <c r="L48" s="13"/>
       <c r="M48" s="14"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" s="12"/>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
@@ -4278,7 +4278,7 @@
       <c r="L49" s="13"/>
       <c r="M49" s="14"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50" s="75"/>
       <c r="C50" s="76"/>
       <c r="D50" s="76"/>
@@ -4294,62 +4294,62 @@
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B30:M30"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="K44:L44"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="K45:L45"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="K46:L46"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="K47:L47"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B30:M30"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="L14:L28">
     <cfRule type="colorScale" priority="2">
@@ -4403,39 +4403,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:O25"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="11.5703125"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="1" max="7" width="11.5546875"/>
+    <col min="8" max="8" width="18.88671875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="11" width="11.5703125"/>
-    <col min="12" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="1025" width="11.5703125"/>
+    <col min="10" max="11" width="11.5546875"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="3:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="144" t="s">
+    <row r="4" spans="3:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="3:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="161" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="144"/>
-      <c r="E5" s="144"/>
-      <c r="F5" s="144"/>
-      <c r="G5" s="144"/>
-      <c r="H5" s="144"/>
-      <c r="I5" s="144"/>
-      <c r="J5" s="144"/>
-      <c r="K5" s="144"/>
-      <c r="L5" s="144"/>
-      <c r="M5" s="144"/>
-      <c r="N5" s="144"/>
-      <c r="O5" s="144"/>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="161"/>
+      <c r="H5" s="161"/>
+      <c r="I5" s="161"/>
+      <c r="J5" s="161"/>
+      <c r="K5" s="161"/>
+      <c r="L5" s="161"/>
+      <c r="M5" s="161"/>
+      <c r="N5" s="161"/>
+      <c r="O5" s="161"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -4450,15 +4450,15 @@
       <c r="N6" s="13"/>
       <c r="O6" s="14"/>
     </row>
-    <row r="7" spans="3:15" ht="33.200000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:15" ht="33.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="12"/>
       <c r="D7" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="145" t="s">
+      <c r="E7" s="162" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="145"/>
+      <c r="F7" s="162"/>
       <c r="G7" s="78" t="s">
         <v>62</v>
       </c>
@@ -4477,23 +4477,23 @@
       <c r="L7" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="145" t="s">
+      <c r="M7" s="162" t="s">
         <v>73</v>
       </c>
-      <c r="N7" s="145"/>
+      <c r="N7" s="162"/>
       <c r="O7" s="14"/>
     </row>
-    <row r="8" spans="3:15" ht="146.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:15" ht="146.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="12"/>
       <c r="D8" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C33</f>
         <v>R1</v>
       </c>
-      <c r="E8" s="146" t="str">
+      <c r="E8" s="160" t="str">
         <f>'Cualitativo y Cuantitativo'!D33</f>
         <v>no trabajar eficientemente</v>
       </c>
-      <c r="F8" s="146"/>
+      <c r="F8" s="160"/>
       <c r="G8" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F33</f>
         <v>MODERADO</v>
@@ -4517,23 +4517,23 @@
         <f>'Cualitativo y Cuantitativo'!J33</f>
         <v>Project Manager</v>
       </c>
-      <c r="M8" s="146" t="s">
+      <c r="M8" s="160" t="s">
         <v>94</v>
       </c>
-      <c r="N8" s="146"/>
+      <c r="N8" s="160"/>
       <c r="O8" s="14"/>
     </row>
-    <row r="9" spans="3:15" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:15" ht="113.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="12"/>
       <c r="D9" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C34</f>
         <v>R2</v>
       </c>
-      <c r="E9" s="146" t="str">
+      <c r="E9" s="160" t="str">
         <f>'Cualitativo y Cuantitativo'!D34</f>
         <v>Tiempos incongruentes y fechas mal planeadas ,Organización ineficiente</v>
       </c>
-      <c r="F9" s="146"/>
+      <c r="F9" s="160"/>
       <c r="G9" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F34</f>
         <v>MODERADO</v>
@@ -4556,23 +4556,23 @@
         <f>'Cualitativo y Cuantitativo'!J34</f>
         <v>Project Manager</v>
       </c>
-      <c r="M9" s="146" t="s">
+      <c r="M9" s="160" t="s">
         <v>103</v>
       </c>
-      <c r="N9" s="146"/>
+      <c r="N9" s="160"/>
       <c r="O9" s="14"/>
     </row>
-    <row r="10" spans="3:15" ht="114.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:15" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="12"/>
       <c r="D10" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C35</f>
         <v>R3</v>
       </c>
-      <c r="E10" s="146" t="str">
+      <c r="E10" s="160" t="str">
         <f>'Cualitativo y Cuantitativo'!D35</f>
         <v>Cambios regulares y nuevos añadidos a los requerimientos</v>
       </c>
-      <c r="F10" s="146"/>
+      <c r="F10" s="160"/>
       <c r="G10" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F35</f>
         <v>MODERADO</v>
@@ -4595,23 +4595,23 @@
         <f>'Cualitativo y Cuantitativo'!J35</f>
         <v>Project Manager</v>
       </c>
-      <c r="M10" s="146" t="s">
+      <c r="M10" s="160" t="s">
         <v>102</v>
       </c>
-      <c r="N10" s="146"/>
+      <c r="N10" s="160"/>
       <c r="O10" s="14"/>
     </row>
-    <row r="11" spans="3:15" ht="92.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:15" ht="92.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="12"/>
       <c r="D11" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C36</f>
         <v>R4</v>
       </c>
-      <c r="E11" s="146" t="str">
+      <c r="E11" s="160" t="str">
         <f>'Cualitativo y Cuantitativo'!D36</f>
         <v>interpretación erronea de las ventanas e interfaces</v>
       </c>
-      <c r="F11" s="146"/>
+      <c r="F11" s="160"/>
       <c r="G11" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F36</f>
         <v>BAJO</v>
@@ -4632,21 +4632,21 @@
       <c r="L11" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="M11" s="146"/>
-      <c r="N11" s="146"/>
+      <c r="M11" s="160"/>
+      <c r="N11" s="160"/>
       <c r="O11" s="14"/>
     </row>
-    <row r="12" spans="3:15" ht="105.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:15" ht="137.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="12"/>
       <c r="D12" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C37</f>
         <v>R5</v>
       </c>
-      <c r="E12" s="146" t="str">
+      <c r="E12" s="160" t="str">
         <f>'Cualitativo y Cuantitativo'!D37</f>
         <v>Estructuración erronea de los datos, tablas mal relacionadas</v>
       </c>
-      <c r="F12" s="146"/>
+      <c r="F12" s="160"/>
       <c r="G12" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F37</f>
         <v>MODERADO</v>
@@ -4669,23 +4669,23 @@
         <f>'Cualitativo y Cuantitativo'!J37</f>
         <v>Project Manager</v>
       </c>
-      <c r="M12" s="146" t="s">
+      <c r="M12" s="160" t="s">
         <v>104</v>
       </c>
-      <c r="N12" s="146"/>
+      <c r="N12" s="160"/>
       <c r="O12" s="14"/>
     </row>
-    <row r="13" spans="3:15" ht="130.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:15" ht="212.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="12"/>
       <c r="D13" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C38</f>
         <v>R6</v>
       </c>
-      <c r="E13" s="146" t="str">
+      <c r="E13" s="160" t="str">
         <f>'Cualitativo y Cuantitativo'!D38</f>
         <v>Pruebas ineficientes</v>
       </c>
-      <c r="F13" s="146"/>
+      <c r="F13" s="160"/>
       <c r="G13" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F38</f>
         <v>ALTO</v>
@@ -4698,7 +4698,7 @@
         <f>Matriz!K21</f>
         <v>•Realizar pruebas completas sobre cada módulo de la aplicación asegurandose de cumplir la funcionalidad principal
 •Darle seguimiento a cada falla encontrado
-•someter nuevs mente a pruebas los módulos donde se reportaron fallas</v>
+•someter nuevamente a pruebas los módulos donde se reportaron fallas</v>
       </c>
       <c r="J13" s="82"/>
       <c r="K13" s="80"/>
@@ -4706,21 +4706,21 @@
         <f>'Cualitativo y Cuantitativo'!J38</f>
         <v>Análista</v>
       </c>
-      <c r="M13" s="146"/>
-      <c r="N13" s="146"/>
+      <c r="M13" s="160"/>
+      <c r="N13" s="160"/>
       <c r="O13" s="14"/>
     </row>
-    <row r="14" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="12"/>
       <c r="D14" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C39</f>
         <v>R7</v>
       </c>
-      <c r="E14" s="146">
+      <c r="E14" s="160">
         <f>'Cualitativo y Cuantitativo'!D39</f>
         <v>0</v>
       </c>
-      <c r="F14" s="146"/>
+      <c r="F14" s="160"/>
       <c r="G14" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F39</f>
         <v>MUY BAJO</v>
@@ -4739,21 +4739,21 @@
         <f>'Cualitativo y Cuantitativo'!J39</f>
         <v>0</v>
       </c>
-      <c r="M14" s="146"/>
-      <c r="N14" s="146"/>
+      <c r="M14" s="160"/>
+      <c r="N14" s="160"/>
       <c r="O14" s="14"/>
     </row>
-    <row r="15" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="12"/>
       <c r="D15" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C40</f>
         <v>R8</v>
       </c>
-      <c r="E15" s="146">
+      <c r="E15" s="160">
         <f>'Cualitativo y Cuantitativo'!D40</f>
         <v>0</v>
       </c>
-      <c r="F15" s="146"/>
+      <c r="F15" s="160"/>
       <c r="G15" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F40</f>
         <v>MUY BAJO</v>
@@ -4772,21 +4772,21 @@
         <f>'Cualitativo y Cuantitativo'!J40</f>
         <v>0</v>
       </c>
-      <c r="M15" s="146"/>
-      <c r="N15" s="146"/>
+      <c r="M15" s="160"/>
+      <c r="N15" s="160"/>
       <c r="O15" s="14"/>
     </row>
-    <row r="16" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="12"/>
       <c r="D16" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C41</f>
         <v>R9</v>
       </c>
-      <c r="E16" s="146">
+      <c r="E16" s="160">
         <f>'Cualitativo y Cuantitativo'!D41</f>
         <v>0</v>
       </c>
-      <c r="F16" s="146"/>
+      <c r="F16" s="160"/>
       <c r="G16" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F41</f>
         <v>MUY BAJO</v>
@@ -4805,21 +4805,21 @@
         <f>'Cualitativo y Cuantitativo'!J41</f>
         <v>0</v>
       </c>
-      <c r="M16" s="146"/>
-      <c r="N16" s="146"/>
+      <c r="M16" s="160"/>
+      <c r="N16" s="160"/>
       <c r="O16" s="14"/>
     </row>
-    <row r="17" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="12"/>
       <c r="D17" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C42</f>
         <v>R10</v>
       </c>
-      <c r="E17" s="146">
+      <c r="E17" s="160">
         <f>'Cualitativo y Cuantitativo'!D42</f>
         <v>0</v>
       </c>
-      <c r="F17" s="146"/>
+      <c r="F17" s="160"/>
       <c r="G17" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F42</f>
         <v>MUY BAJO</v>
@@ -4838,21 +4838,21 @@
         <f>'Cualitativo y Cuantitativo'!J42</f>
         <v>0</v>
       </c>
-      <c r="M17" s="146"/>
-      <c r="N17" s="146"/>
+      <c r="M17" s="160"/>
+      <c r="N17" s="160"/>
       <c r="O17" s="14"/>
     </row>
-    <row r="18" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="12"/>
       <c r="D18" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C43</f>
         <v>R11</v>
       </c>
-      <c r="E18" s="146">
+      <c r="E18" s="160">
         <f>'Cualitativo y Cuantitativo'!D43</f>
         <v>0</v>
       </c>
-      <c r="F18" s="146"/>
+      <c r="F18" s="160"/>
       <c r="G18" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F43</f>
         <v>MUY BAJO</v>
@@ -4871,21 +4871,21 @@
         <f>'Cualitativo y Cuantitativo'!J43</f>
         <v>0</v>
       </c>
-      <c r="M18" s="146"/>
-      <c r="N18" s="146"/>
+      <c r="M18" s="160"/>
+      <c r="N18" s="160"/>
       <c r="O18" s="14"/>
     </row>
-    <row r="19" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="12"/>
       <c r="D19" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C44</f>
         <v>R12</v>
       </c>
-      <c r="E19" s="146">
+      <c r="E19" s="160">
         <f>'Cualitativo y Cuantitativo'!D44</f>
         <v>0</v>
       </c>
-      <c r="F19" s="146"/>
+      <c r="F19" s="160"/>
       <c r="G19" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F44</f>
         <v>MUY BAJO</v>
@@ -4904,21 +4904,21 @@
         <f>'Cualitativo y Cuantitativo'!J44</f>
         <v>0</v>
       </c>
-      <c r="M19" s="146"/>
-      <c r="N19" s="146"/>
+      <c r="M19" s="160"/>
+      <c r="N19" s="160"/>
       <c r="O19" s="14"/>
     </row>
-    <row r="20" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="12"/>
       <c r="D20" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C45</f>
         <v>R13</v>
       </c>
-      <c r="E20" s="146">
+      <c r="E20" s="160">
         <f>'Cualitativo y Cuantitativo'!D45</f>
         <v>0</v>
       </c>
-      <c r="F20" s="146"/>
+      <c r="F20" s="160"/>
       <c r="G20" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F45</f>
         <v>MUY BAJO</v>
@@ -4937,21 +4937,21 @@
         <f>'Cualitativo y Cuantitativo'!J45</f>
         <v>0</v>
       </c>
-      <c r="M20" s="146"/>
-      <c r="N20" s="146"/>
+      <c r="M20" s="160"/>
+      <c r="N20" s="160"/>
       <c r="O20" s="14"/>
     </row>
-    <row r="21" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="12"/>
       <c r="D21" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C46</f>
         <v>R14</v>
       </c>
-      <c r="E21" s="146">
+      <c r="E21" s="160">
         <f>'Cualitativo y Cuantitativo'!D46</f>
         <v>0</v>
       </c>
-      <c r="F21" s="146"/>
+      <c r="F21" s="160"/>
       <c r="G21" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F46</f>
         <v>MUY BAJO</v>
@@ -4970,21 +4970,21 @@
         <f>'Cualitativo y Cuantitativo'!J46</f>
         <v>0</v>
       </c>
-      <c r="M21" s="146"/>
-      <c r="N21" s="146"/>
+      <c r="M21" s="160"/>
+      <c r="N21" s="160"/>
       <c r="O21" s="14"/>
     </row>
-    <row r="22" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="12"/>
       <c r="D22" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C47</f>
         <v>R15</v>
       </c>
-      <c r="E22" s="146">
+      <c r="E22" s="160">
         <f>'Cualitativo y Cuantitativo'!D47</f>
         <v>0</v>
       </c>
-      <c r="F22" s="146"/>
+      <c r="F22" s="160"/>
       <c r="G22" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F47</f>
         <v>MUY BAJO</v>
@@ -5003,11 +5003,11 @@
         <f>'Cualitativo y Cuantitativo'!J47</f>
         <v>0</v>
       </c>
-      <c r="M22" s="146"/>
-      <c r="N22" s="146"/>
+      <c r="M22" s="160"/>
+      <c r="N22" s="160"/>
       <c r="O22" s="14"/>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
@@ -5022,7 +5022,7 @@
       <c r="N23" s="13"/>
       <c r="O23" s="14"/>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" s="12"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
@@ -5037,7 +5037,7 @@
       <c r="N24" s="13"/>
       <c r="O24" s="14"/>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" s="75"/>
       <c r="D25" s="76"/>
       <c r="E25" s="76"/>
@@ -5054,6 +5054,29 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C5:O5"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="M17:N17"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="E22:F22"/>
@@ -5064,29 +5087,6 @@
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="C5:O5"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="M8:N8"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5117,18 +5117,18 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="3.28515625" customWidth="1"/>
-    <col min="3" max="8" width="7.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" customWidth="1"/>
-    <col min="11" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" customWidth="1"/>
+    <col min="3" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" customWidth="1"/>
+    <col min="11" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="147" t="s">
+    <row r="5" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="163" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="83">
@@ -5160,8 +5160,8 @@
       <c r="M5" s="84"/>
       <c r="N5" s="84"/>
     </row>
-    <row r="6" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="147"/>
+    <row r="6" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="163"/>
       <c r="C6" s="83">
         <v>4</v>
       </c>
@@ -5191,8 +5191,8 @@
       <c r="M6" s="84"/>
       <c r="N6" s="84"/>
     </row>
-    <row r="7" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="147"/>
+    <row r="7" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="163"/>
       <c r="C7" s="83">
         <v>3</v>
       </c>
@@ -5222,8 +5222,8 @@
       <c r="M7" s="84"/>
       <c r="N7" s="84"/>
     </row>
-    <row r="8" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="147"/>
+    <row r="8" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="163"/>
       <c r="C8" s="83">
         <v>2</v>
       </c>
@@ -5253,8 +5253,8 @@
       <c r="M8" s="84"/>
       <c r="N8" s="84"/>
     </row>
-    <row r="9" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="147"/>
+    <row r="9" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="163"/>
       <c r="C9" s="83">
         <v>1</v>
       </c>
@@ -5284,7 +5284,7 @@
       <c r="M9" s="84"/>
       <c r="N9" s="84"/>
     </row>
-    <row r="10" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="85"/>
       <c r="D10" s="86">
         <v>1</v>
@@ -5302,14 +5302,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D11" s="148" t="s">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D11" s="164" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="148"/>
-      <c r="F11" s="148"/>
-      <c r="G11" s="148"/>
-      <c r="H11" s="148"/>
+      <c r="E11" s="164"/>
+      <c r="F11" s="164"/>
+      <c r="G11" s="164"/>
+      <c r="H11" s="164"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5333,21 +5333,21 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1025" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D6" s="149" t="s">
+    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="165" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="149"/>
+      <c r="E6" s="165"/>
       <c r="G6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D7" s="87" t="s">
         <v>67</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D8" s="88" t="s">
         <v>75</v>
       </c>
@@ -5365,13 +5365,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" s="88" t="s">
         <v>77</v>
       </c>
       <c r="E9" s="88"/>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" s="88" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
actualizacion de la plan de gestion de riesgos 1.1
</commit_message>
<xml_diff>
--- a/Entregables/V. Análisis de riesgo del proyecto de TI/APPMO-SP_ARP_v1.1.xlsx
+++ b/Entregables/V. Análisis de riesgo del proyecto de TI/APPMO-SP_ARP_v1.1.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FRANC\Desktop\SM-ROOT\Entregables\V. Análisis de riesgo del proyecto de TI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cecy Tapia\Desktop\SM-ROOT\Entregables\V. Análisis de riesgo del proyecto de TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz" sheetId="1" r:id="rId1"/>
-    <sheet name="Cualitativo y Cuantitativo" sheetId="2" r:id="rId2"/>
+    <sheet name="Cualitativo " sheetId="2" r:id="rId2"/>
     <sheet name="Plan de contingencia" sheetId="3" r:id="rId3"/>
     <sheet name="Grafica" sheetId="4" r:id="rId4"/>
     <sheet name="Datos" sheetId="5" r:id="rId5"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="133">
   <si>
     <t>Probabilidad</t>
   </si>
@@ -350,9 +350,6 @@
     <t>Retrazo de avances con el software</t>
   </si>
   <si>
-    <t>Todos los miembros del equipo de trabajo tienen acceso al repositorio creado</t>
-  </si>
-  <si>
     <t>Pruebas</t>
   </si>
   <si>
@@ -369,18 +366,6 @@
   </si>
   <si>
     <t>Codificiación</t>
-  </si>
-  <si>
-    <t>Análista</t>
-  </si>
-  <si>
-    <t>Los nuevos cambios a los requisitos se acomplan a los ya dados antes.</t>
-  </si>
-  <si>
-    <t>Se crea un diagrama de las actividades y tiempos</t>
-  </si>
-  <si>
-    <t>La estructura es diferente a los diseños, al ser un software móvil, su propia naturaleza afecta a la codificación misma.</t>
   </si>
   <si>
     <t>Mal entendimiento de los requerimientos</t>
@@ -418,9 +403,6 @@
   </si>
   <si>
     <t>Revisar actividades con fechas y ajustarlos a tiempos del proyecto, utilizar un repositorio para el almacenamiento de la información.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acoplar los requerimientos nuevos cambios o existentes de forma clara y  eficiente  para cumplir la funcionalidad planeada </t>
   </si>
   <si>
     <t>interpretación erronea de las ventanas e interfaces</t>
@@ -453,6 +435,39 @@
     <t>•Realizar pruebas completas sobre cada módulo de la aplicación asegurandose de cumplir la funcionalidad principal
 •Darle seguimiento a cada falla encontrado
 •someter nuevamente a pruebas los módulos donde se reportaron fallas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acoplar los requerimientos nuevos o cambios  existentes de forma clara y  eficiente  para cumplir la funcionalidad planeada </t>
+  </si>
+  <si>
+    <t>Comunicación</t>
+  </si>
+  <si>
+    <t>todos los entregables del proyecto</t>
+  </si>
+  <si>
+    <t>Portafolio manager</t>
+  </si>
+  <si>
+    <t>todas las  minutas de trabajo se encuentra programado como parte de la agenda el punto de acuerdos, para establecer fechas, responsables, actividades y seguimiento de las tareas pendientes.</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>programador</t>
+  </si>
+  <si>
+    <t>Se restructuró  el cronograma que las  actividades y tiempos, se reajusten y coincidan.</t>
+  </si>
+  <si>
+    <t>Los nuevos cambios a los requisitos se ajustan  a los anteriores.</t>
+  </si>
+  <si>
+    <t>nuevo analisis de los datos para  el rediseño de las intefaces ajustandola a los nuevos datos en la base de datos.</t>
+  </si>
+  <si>
+    <t>nueva estructura de los datos  ajustando la base de datos de forma que se ajustaron los nuevos datos al diseño existente</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1376,9 +1391,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1596,6 +1608,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1694,6 +1712,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2045,41 +2066,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K34"/>
   <sheetViews>
-    <sheetView topLeftCell="B14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="D12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" customWidth="1"/>
-    <col min="9" max="9" width="7.5546875" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
-    <col min="12" max="1023" width="8.5546875" customWidth="1"/>
+    <col min="12" max="1023" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="134" t="s">
+    <row r="1" spans="2:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="135" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="135"/>
-      <c r="K1" s="136"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="137"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="26"/>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2091,7 +2112,7 @@
       <c r="J2" s="27"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="2:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2103,23 +2124,23 @@
       <c r="J3" s="13"/>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="141" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="142" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
       <c r="E4" s="13"/>
-      <c r="F4" s="141" t="s">
+      <c r="F4" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="141"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="141"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
       <c r="J4" s="13"/>
       <c r="K4" s="14"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>5</v>
       </c>
@@ -2136,14 +2157,14 @@
       <c r="G5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="137" t="s">
+      <c r="H5" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="137"/>
+      <c r="I5" s="138"/>
       <c r="J5" s="13"/>
       <c r="K5" s="14"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -2160,14 +2181,14 @@
       <c r="G6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="137" t="s">
+      <c r="H6" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="137"/>
+      <c r="I6" s="138"/>
       <c r="J6" s="13"/>
       <c r="K6" s="14"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>3</v>
       </c>
@@ -2184,14 +2205,14 @@
       <c r="G7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="137" t="s">
+      <c r="H7" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="137"/>
+      <c r="I7" s="138"/>
       <c r="J7" s="13"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>2</v>
       </c>
@@ -2208,14 +2229,14 @@
       <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="137" t="s">
+      <c r="H8" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="137"/>
+      <c r="I8" s="138"/>
       <c r="J8" s="13"/>
       <c r="K8" s="14"/>
     </row>
-    <row r="9" spans="2:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>1</v>
       </c>
@@ -2232,14 +2253,14 @@
       <c r="G9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="138" t="s">
+      <c r="H9" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="138"/>
+      <c r="I9" s="139"/>
       <c r="J9" s="13"/>
       <c r="K9" s="14"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -2251,7 +2272,7 @@
       <c r="J10" s="13"/>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -2263,7 +2284,7 @@
       <c r="J11" s="13"/>
       <c r="K11" s="14"/>
     </row>
-    <row r="12" spans="2:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -2275,19 +2296,19 @@
       <c r="J12" s="13"/>
       <c r="K12" s="14"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="139" t="s">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="140" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="139"/>
-      <c r="D13" s="139"/>
-      <c r="E13" s="139"/>
-      <c r="F13" s="139"/>
-      <c r="G13" s="139"/>
-      <c r="H13" s="140" t="s">
+      <c r="C13" s="140"/>
+      <c r="D13" s="140"/>
+      <c r="E13" s="140"/>
+      <c r="F13" s="140"/>
+      <c r="G13" s="140"/>
+      <c r="H13" s="141" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="140"/>
+      <c r="I13" s="141"/>
       <c r="J13" s="8" t="s">
         <v>23</v>
       </c>
@@ -2295,19 +2316,19 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="133"/>
-      <c r="C14" s="133"/>
-      <c r="D14" s="133"/>
-      <c r="E14" s="133"/>
-      <c r="F14" s="133"/>
-      <c r="G14" s="133"/>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="134"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="134"/>
+      <c r="E14" s="134"/>
+      <c r="F14" s="134"/>
+      <c r="G14" s="134"/>
       <c r="H14" s="9"/>
       <c r="I14" s="10"/>
       <c r="J14" s="11"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
         <v>24</v>
       </c>
@@ -2335,398 +2356,398 @@
       <c r="J15" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="102" t="s">
+      <c r="K15" s="101" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="98">
+    <row r="16" spans="2:11" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="97">
         <v>1</v>
       </c>
-      <c r="C16" s="99" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="121" t="s">
+      <c r="C16" s="98" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" s="120" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="121" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="122" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="123" t="s">
+        <v>107</v>
+      </c>
+      <c r="H16" s="108">
+        <v>3</v>
+      </c>
+      <c r="I16" s="108">
+        <v>5</v>
+      </c>
+      <c r="J16" s="109">
+        <f t="shared" ref="J16:J30" si="0">H16*I16</f>
+        <v>15</v>
+      </c>
+      <c r="K16" s="116" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="122" t="s">
-        <v>110</v>
-      </c>
-      <c r="F16" s="123" t="s">
-        <v>111</v>
-      </c>
-      <c r="G16" s="124" t="s">
-        <v>112</v>
-      </c>
-      <c r="H16" s="109">
-        <v>3</v>
-      </c>
-      <c r="I16" s="109">
-        <v>4</v>
-      </c>
-      <c r="J16" s="110">
-        <f t="shared" ref="J16:J30" si="0">H16*I16</f>
-        <v>12</v>
-      </c>
-      <c r="K16" s="117" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="20">
         <v>2</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="125" t="s">
-        <v>107</v>
-      </c>
-      <c r="E17" s="126" t="s">
+      <c r="D17" s="124" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="125" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="126" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="127" t="s">
-        <v>114</v>
-      </c>
-      <c r="G17" s="128" t="s">
-        <v>115</v>
-      </c>
-      <c r="H17" s="111">
+      <c r="G17" s="127" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17" s="110">
         <v>3</v>
       </c>
-      <c r="I17" s="111">
+      <c r="I17" s="110">
         <v>4</v>
       </c>
-      <c r="J17" s="112">
+      <c r="J17" s="111">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="K17" s="118" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="117" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="22">
         <v>3</v>
       </c>
       <c r="C18" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="129" t="s">
+      <c r="D18" s="128" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="130" t="s">
+      <c r="E18" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="131" t="s">
+      <c r="F18" s="130" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="132" t="s">
+      <c r="G18" s="131" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="113">
+      <c r="H18" s="112">
         <v>3</v>
       </c>
-      <c r="I18" s="113">
+      <c r="I18" s="112">
         <v>4</v>
       </c>
-      <c r="J18" s="114">
+      <c r="J18" s="113">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="K18" s="119" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" ht="70.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="118" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="22">
         <v>4</v>
       </c>
       <c r="C19" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="129" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19" s="130" t="s">
-        <v>118</v>
-      </c>
-      <c r="F19" s="131" t="s">
-        <v>120</v>
-      </c>
-      <c r="G19" s="132" t="s">
-        <v>119</v>
-      </c>
-      <c r="H19" s="113">
+      <c r="D19" s="128" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="129" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="130" t="s">
+        <v>114</v>
+      </c>
+      <c r="G19" s="131" t="s">
+        <v>113</v>
+      </c>
+      <c r="H19" s="112">
         <v>2</v>
       </c>
-      <c r="I19" s="113">
+      <c r="I19" s="112">
         <v>3</v>
       </c>
-      <c r="J19" s="114">
+      <c r="J19" s="113">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K19" s="120" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="119" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="22">
         <v>5</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="129" t="s">
-        <v>122</v>
-      </c>
-      <c r="E20" s="130" t="s">
-        <v>123</v>
-      </c>
-      <c r="F20" s="131" t="s">
-        <v>125</v>
-      </c>
-      <c r="G20" s="132" t="s">
-        <v>124</v>
-      </c>
-      <c r="H20" s="113">
+      <c r="D20" s="128" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="129" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="130" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="131" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" s="112">
         <v>3</v>
       </c>
-      <c r="I20" s="113">
+      <c r="I20" s="112">
         <v>4</v>
       </c>
-      <c r="J20" s="114">
+      <c r="J20" s="113">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="K20" s="120" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="119" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="22">
         <v>6</v>
       </c>
       <c r="C21" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="128" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="129" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="130" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="131" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="129" t="s">
-        <v>97</v>
-      </c>
-      <c r="E21" s="130" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="131" t="s">
-        <v>106</v>
-      </c>
-      <c r="G21" s="132" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="113">
+      <c r="H21" s="112">
         <v>3</v>
       </c>
-      <c r="I21" s="113">
+      <c r="I21" s="112">
         <v>5</v>
       </c>
-      <c r="J21" s="114">
+      <c r="J21" s="113">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="K21" s="119" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="118" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="22">
         <v>7</v>
       </c>
       <c r="C22" s="23"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="92"/>
-      <c r="F22" s="94"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="113">
-        <v>0</v>
-      </c>
-      <c r="I22" s="113">
-        <v>0</v>
-      </c>
-      <c r="J22" s="114">
+      <c r="D22" s="89"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="95"/>
+      <c r="H22" s="112">
+        <v>0</v>
+      </c>
+      <c r="I22" s="112">
+        <v>0</v>
+      </c>
+      <c r="J22" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K22" s="100"/>
-    </row>
-    <row r="23" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="99"/>
+    </row>
+    <row r="23" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="22">
         <v>8</v>
       </c>
       <c r="C23" s="23"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="92"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="113">
-        <v>0</v>
-      </c>
-      <c r="I23" s="113">
-        <v>0</v>
-      </c>
-      <c r="J23" s="114">
+      <c r="D23" s="89"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="95"/>
+      <c r="H23" s="112">
+        <v>0</v>
+      </c>
+      <c r="I23" s="112">
+        <v>0</v>
+      </c>
+      <c r="J23" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K23" s="100"/>
-    </row>
-    <row r="24" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="99"/>
+    </row>
+    <row r="24" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="22">
         <v>9</v>
       </c>
       <c r="C24" s="23"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="92"/>
-      <c r="F24" s="94"/>
-      <c r="G24" s="96"/>
-      <c r="H24" s="113">
-        <v>0</v>
-      </c>
-      <c r="I24" s="113">
-        <v>0</v>
-      </c>
-      <c r="J24" s="114">
+      <c r="D24" s="89"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="112">
+        <v>0</v>
+      </c>
+      <c r="I24" s="112">
+        <v>0</v>
+      </c>
+      <c r="J24" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K24" s="100"/>
-    </row>
-    <row r="25" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K24" s="99"/>
+    </row>
+    <row r="25" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="22">
         <v>10</v>
       </c>
       <c r="C25" s="23"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="92"/>
-      <c r="F25" s="94"/>
-      <c r="G25" s="96"/>
-      <c r="H25" s="113">
-        <v>0</v>
-      </c>
-      <c r="I25" s="113">
-        <v>0</v>
-      </c>
-      <c r="J25" s="114">
+      <c r="D25" s="89"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="95"/>
+      <c r="H25" s="112">
+        <v>0</v>
+      </c>
+      <c r="I25" s="112">
+        <v>0</v>
+      </c>
+      <c r="J25" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K25" s="100"/>
-    </row>
-    <row r="26" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="99"/>
+    </row>
+    <row r="26" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="22">
         <v>11</v>
       </c>
       <c r="C26" s="23"/>
-      <c r="D26" s="90"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="94"/>
-      <c r="G26" s="96"/>
-      <c r="H26" s="113">
-        <v>0</v>
-      </c>
-      <c r="I26" s="113">
-        <v>0</v>
-      </c>
-      <c r="J26" s="114">
+      <c r="D26" s="89"/>
+      <c r="E26" s="91"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="112">
+        <v>0</v>
+      </c>
+      <c r="I26" s="112">
+        <v>0</v>
+      </c>
+      <c r="J26" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K26" s="100"/>
-    </row>
-    <row r="27" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K26" s="99"/>
+    </row>
+    <row r="27" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="22">
         <v>12</v>
       </c>
       <c r="C27" s="23"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="92"/>
-      <c r="F27" s="94"/>
-      <c r="G27" s="96"/>
-      <c r="H27" s="113">
-        <v>0</v>
-      </c>
-      <c r="I27" s="113">
-        <v>0</v>
-      </c>
-      <c r="J27" s="114">
+      <c r="D27" s="89"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="112">
+        <v>0</v>
+      </c>
+      <c r="I27" s="112">
+        <v>0</v>
+      </c>
+      <c r="J27" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K27" s="100"/>
-    </row>
-    <row r="28" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="99"/>
+    </row>
+    <row r="28" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="22">
         <v>13</v>
       </c>
       <c r="C28" s="23"/>
-      <c r="D28" s="90"/>
-      <c r="E28" s="92"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="113">
-        <v>0</v>
-      </c>
-      <c r="I28" s="113">
-        <v>0</v>
-      </c>
-      <c r="J28" s="114">
+      <c r="D28" s="89"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="112">
+        <v>0</v>
+      </c>
+      <c r="I28" s="112">
+        <v>0</v>
+      </c>
+      <c r="J28" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K28" s="100"/>
-    </row>
-    <row r="29" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="99"/>
+    </row>
+    <row r="29" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="22">
         <v>14</v>
       </c>
       <c r="C29" s="23"/>
-      <c r="D29" s="90"/>
-      <c r="E29" s="92"/>
-      <c r="F29" s="94"/>
-      <c r="G29" s="96"/>
-      <c r="H29" s="113">
-        <v>0</v>
-      </c>
-      <c r="I29" s="113">
-        <v>0</v>
-      </c>
-      <c r="J29" s="114">
+      <c r="D29" s="89"/>
+      <c r="E29" s="91"/>
+      <c r="F29" s="93"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="112">
+        <v>0</v>
+      </c>
+      <c r="I29" s="112">
+        <v>0</v>
+      </c>
+      <c r="J29" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K29" s="100"/>
-    </row>
-    <row r="30" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K29" s="99"/>
+    </row>
+    <row r="30" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="24">
         <v>15</v>
       </c>
       <c r="C30" s="25"/>
-      <c r="D30" s="91"/>
-      <c r="E30" s="93"/>
-      <c r="F30" s="95"/>
-      <c r="G30" s="97"/>
-      <c r="H30" s="115">
-        <v>0</v>
-      </c>
-      <c r="I30" s="115">
-        <v>0</v>
-      </c>
-      <c r="J30" s="116">
+      <c r="D30" s="90"/>
+      <c r="E30" s="92"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="96"/>
+      <c r="H30" s="114">
+        <v>0</v>
+      </c>
+      <c r="I30" s="114">
+        <v>0</v>
+      </c>
+      <c r="J30" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K30" s="101"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K30" s="100"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -2738,7 +2759,7 @@
       <c r="J31" s="13"/>
       <c r="K31" s="14"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="12"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -2750,7 +2771,7 @@
       <c r="J32" s="13"/>
       <c r="K32" s="14"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -2762,17 +2783,17 @@
       <c r="J33" s="13"/>
       <c r="K33" s="14"/>
     </row>
-    <row r="34" spans="2:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="75"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="76"/>
-      <c r="G34" s="76"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="76"/>
-      <c r="J34" s="76"/>
-      <c r="K34" s="77"/>
+    <row r="34" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="74"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2801,24 +2822,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" s="26"/>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2832,23 +2853,23 @@
       <c r="L2" s="27"/>
       <c r="M2" s="28"/>
     </row>
-    <row r="3" spans="2:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="157" t="s">
+      <c r="C3" s="158" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
-      <c r="F3" s="157"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="157"/>
-      <c r="L3" s="157"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
+      <c r="L3" s="158"/>
       <c r="M3" s="14"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -2862,7 +2883,7 @@
       <c r="L4" s="13"/>
       <c r="M4" s="14"/>
     </row>
-    <row r="5" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
       <c r="C5" s="29" t="s">
         <v>0</v>
@@ -2881,16 +2902,16 @@
       <c r="I5" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="158" t="s">
+      <c r="J5" s="159" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="158"/>
+      <c r="K5" s="159"/>
       <c r="L5" s="34" t="s">
         <v>36</v>
       </c>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="2:17" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="12"/>
       <c r="C6" s="35" t="s">
         <v>37</v>
@@ -2909,17 +2930,17 @@
       <c r="I6" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="159" t="s">
+      <c r="J6" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="159"/>
+      <c r="K6" s="160"/>
       <c r="L6" s="37">
         <f>16/25*100</f>
         <v>64</v>
       </c>
       <c r="M6" s="14"/>
     </row>
-    <row r="7" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="12"/>
       <c r="C7" s="40" t="s">
         <v>41</v>
@@ -2938,17 +2959,17 @@
       <c r="I7" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="153" t="s">
+      <c r="J7" s="154" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="153"/>
+      <c r="K7" s="154"/>
       <c r="L7" s="42">
         <f>15/25*100</f>
         <v>60</v>
       </c>
       <c r="M7" s="14"/>
     </row>
-    <row r="8" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12"/>
       <c r="C8" s="40" t="s">
         <v>45</v>
@@ -2967,17 +2988,17 @@
       <c r="I8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="153" t="s">
+      <c r="J8" s="154" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="153"/>
+      <c r="K8" s="154"/>
       <c r="L8" s="42">
         <f>12/25*100</f>
         <v>48</v>
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12"/>
       <c r="C9" s="40" t="s">
         <v>47</v>
@@ -2996,17 +3017,17 @@
       <c r="I9" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="153" t="s">
+      <c r="J9" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="153"/>
+      <c r="K9" s="154"/>
       <c r="L9" s="42">
         <f>8/25*100</f>
         <v>32</v>
       </c>
       <c r="M9" s="14"/>
     </row>
-    <row r="10" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
       <c r="C10" s="45" t="s">
         <v>49</v>
@@ -3025,10 +3046,10 @@
       <c r="I10" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="154" t="s">
+      <c r="J10" s="155" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="154"/>
+      <c r="K10" s="155"/>
       <c r="L10" s="47">
         <f>5/25*100</f>
         <v>20</v>
@@ -3039,7 +3060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
       <c r="C11" s="49"/>
       <c r="D11" s="13"/>
@@ -3053,7 +3074,7 @@
       <c r="L11" s="13"/>
       <c r="M11" s="14"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -3067,17 +3088,17 @@
       <c r="L12" s="13"/>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="2:17" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="155" t="s">
+      <c r="D13" s="156" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="155"/>
+      <c r="E13" s="156"/>
       <c r="F13" s="51" t="s">
         <v>54</v>
       </c>
@@ -3101,587 +3122,589 @@
       </c>
       <c r="M13" s="14"/>
     </row>
-    <row r="14" spans="2:17" ht="88.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" ht="88.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="12"/>
       <c r="C14" s="53" t="str">
         <f>CONCATENATE($B$13,Matriz!B16)</f>
         <v>R1</v>
       </c>
-      <c r="D14" s="156" t="str">
+      <c r="D14" s="157" t="str">
         <f>Matriz!E16</f>
         <v>no trabajar eficientemente</v>
       </c>
-      <c r="E14" s="156"/>
+      <c r="E14" s="157"/>
       <c r="F14" s="54" t="str">
         <f>Matriz!F16</f>
         <v xml:space="preserve">Mala comunicación, descuerdos en el equipo y trabajo disperso. </v>
       </c>
-      <c r="G14" s="55"/>
+      <c r="G14" s="132" t="s">
+        <v>124</v>
+      </c>
       <c r="H14" s="54">
         <f>Matriz!H16</f>
         <v>3</v>
       </c>
       <c r="I14" s="54">
         <f>Matriz!I16</f>
-        <v>4</v>
-      </c>
-      <c r="J14" s="56">
+        <v>5</v>
+      </c>
+      <c r="J14" s="55">
         <f t="shared" ref="J14:J28" si="0">H14*I14</f>
-        <v>12</v>
-      </c>
-      <c r="K14" s="56" t="str">
+        <v>15</v>
+      </c>
+      <c r="K14" s="55" t="str">
         <f t="shared" ref="K14:K28" si="1">IF(J14&lt;5,"MUY BAJO",IF( AND(J14&gt;=5,J14&lt;8),"BAJO",IF(AND(J14&gt;=8,J14&lt;=12),"MODERADO",IF(AND(J14&gt;=12,J14&lt;=15),"ALTO","MUY ALTO"))))</f>
-        <v>MODERADO</v>
-      </c>
-      <c r="L14" s="57">
+        <v>ALTO</v>
+      </c>
+      <c r="L14" s="56">
         <f t="shared" ref="L14:L28" si="2">J14/25*100</f>
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="2:17" ht="79.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="12"/>
       <c r="C15" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B17)</f>
         <v>R2</v>
       </c>
-      <c r="D15" s="149" t="str">
+      <c r="D15" s="150" t="str">
         <f>Matriz!E17</f>
         <v>Tiempos incongruentes y fechas mal planeadas ,Organización ineficiente</v>
       </c>
-      <c r="E15" s="149"/>
-      <c r="F15" s="58" t="str">
+      <c r="E15" s="150"/>
+      <c r="F15" s="57" t="str">
         <f>Matriz!F17</f>
         <v xml:space="preserve"> Retrazo en entregables del proyecto e información dispersa</v>
       </c>
-      <c r="G15" s="107" t="s">
+      <c r="G15" s="106" t="s">
         <v>84</v>
       </c>
-      <c r="H15" s="58">
+      <c r="H15" s="57">
         <f>Matriz!H17</f>
         <v>3</v>
       </c>
-      <c r="I15" s="58">
+      <c r="I15" s="57">
         <f>Matriz!I17</f>
         <v>4</v>
       </c>
-      <c r="J15" s="60">
+      <c r="J15" s="59">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="K15" s="60" t="str">
+      <c r="K15" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MODERADO</v>
       </c>
-      <c r="L15" s="61">
+      <c r="L15" s="60">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="M15" s="14"/>
     </row>
-    <row r="16" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="12"/>
       <c r="C16" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B18)</f>
         <v>R3</v>
       </c>
-      <c r="D16" s="149" t="str">
+      <c r="D16" s="150" t="str">
         <f>Matriz!E18</f>
         <v>Cambios regulares y nuevos añadidos a los requerimientos</v>
       </c>
-      <c r="E16" s="149"/>
-      <c r="F16" s="107" t="str">
+      <c r="E16" s="150"/>
+      <c r="F16" s="106" t="str">
         <f>Matriz!F18</f>
         <v>Requerimientos ambiguos o incompletos</v>
       </c>
-      <c r="G16" s="107" t="s">
-        <v>99</v>
-      </c>
-      <c r="H16" s="58">
+      <c r="G16" s="106" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="57">
         <f>Matriz!H18</f>
         <v>3</v>
       </c>
-      <c r="I16" s="58">
+      <c r="I16" s="57">
         <f>Matriz!I18</f>
         <v>4</v>
       </c>
-      <c r="J16" s="60">
+      <c r="J16" s="59">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="K16" s="60" t="str">
+      <c r="K16" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MODERADO</v>
       </c>
-      <c r="L16" s="61">
+      <c r="L16" s="60">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:13" ht="86.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="86.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="12"/>
       <c r="C17" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B19)</f>
         <v>R4</v>
       </c>
-      <c r="D17" s="149" t="str">
+      <c r="D17" s="150" t="str">
         <f>Matriz!E19</f>
         <v>interpretación erronea de las ventanas e interfaces</v>
       </c>
-      <c r="E17" s="149"/>
-      <c r="F17" s="107" t="str">
+      <c r="E17" s="150"/>
+      <c r="F17" s="106" t="str">
         <f>Matriz!F19</f>
         <v>Diseño de interfaces equivocadas o mal diseñadas</v>
       </c>
-      <c r="G17" s="107" t="s">
+      <c r="G17" s="106" t="s">
         <v>91</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="57">
         <f>Matriz!H19</f>
         <v>2</v>
       </c>
-      <c r="I17" s="58">
+      <c r="I17" s="57">
         <f>Matriz!I19</f>
         <v>3</v>
       </c>
-      <c r="J17" s="60">
+      <c r="J17" s="59">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K17" s="60" t="str">
+      <c r="K17" s="59" t="str">
         <f t="shared" si="1"/>
         <v>BAJO</v>
       </c>
-      <c r="L17" s="61">
+      <c r="L17" s="60">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="M17" s="14"/>
     </row>
-    <row r="18" spans="2:13" ht="95.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="95.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="12"/>
       <c r="C18" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B20)</f>
         <v>R5</v>
       </c>
-      <c r="D18" s="149" t="str">
+      <c r="D18" s="150" t="str">
         <f>Matriz!E20</f>
         <v>Estructuración erronea de los datos, tablas mal relacionadas</v>
       </c>
-      <c r="E18" s="149"/>
-      <c r="F18" s="58" t="str">
+      <c r="E18" s="150"/>
+      <c r="F18" s="57" t="str">
         <f>Matriz!F20</f>
         <v>Retrazo en codificación del producto</v>
       </c>
-      <c r="G18" s="59" t="s">
-        <v>100</v>
-      </c>
-      <c r="H18" s="58">
+      <c r="G18" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" s="57">
         <f>Matriz!H20</f>
         <v>3</v>
       </c>
-      <c r="I18" s="58">
+      <c r="I18" s="57">
         <f>Matriz!I20</f>
         <v>4</v>
       </c>
-      <c r="J18" s="60">
+      <c r="J18" s="59">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="K18" s="60" t="str">
+      <c r="K18" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MODERADO</v>
       </c>
-      <c r="L18" s="61">
+      <c r="L18" s="60">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:13" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="12"/>
       <c r="C19" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B21)</f>
         <v>R6</v>
       </c>
-      <c r="D19" s="149" t="str">
+      <c r="D19" s="150" t="str">
         <f>Matriz!E21</f>
         <v>Pruebas ineficientes</v>
       </c>
-      <c r="E19" s="149"/>
-      <c r="F19" s="58" t="str">
+      <c r="E19" s="150"/>
+      <c r="F19" s="57" t="str">
         <f>Matriz!F21</f>
         <v>Mala ejecución del producto, presenta errores</v>
       </c>
-      <c r="G19" s="59" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" s="58">
+      <c r="G19" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="H19" s="57">
         <f>Matriz!H21</f>
         <v>3</v>
       </c>
-      <c r="I19" s="58">
+      <c r="I19" s="57">
         <f>Matriz!I21</f>
         <v>5</v>
       </c>
-      <c r="J19" s="60">
+      <c r="J19" s="59">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="K19" s="60" t="str">
+      <c r="K19" s="59" t="str">
         <f t="shared" si="1"/>
         <v>ALTO</v>
       </c>
-      <c r="L19" s="61">
+      <c r="L19" s="60">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="12"/>
       <c r="C20" s="53" t="str">
         <f>CONCATENATE($B$13,Matriz!B22)</f>
         <v>R7</v>
       </c>
-      <c r="D20" s="149">
+      <c r="D20" s="150">
         <f>Matriz!E22</f>
         <v>0</v>
       </c>
-      <c r="E20" s="149"/>
-      <c r="F20" s="58">
+      <c r="E20" s="150"/>
+      <c r="F20" s="57">
         <f>Matriz!F22</f>
         <v>0</v>
       </c>
-      <c r="G20" s="59"/>
-      <c r="H20" s="58">
+      <c r="G20" s="58"/>
+      <c r="H20" s="57">
         <f>Matriz!H22</f>
         <v>0</v>
       </c>
-      <c r="I20" s="58">
+      <c r="I20" s="57">
         <f>Matriz!I22</f>
         <v>0</v>
       </c>
-      <c r="J20" s="60">
+      <c r="J20" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K20" s="60" t="str">
+      <c r="K20" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="L20" s="61">
+      <c r="L20" s="60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M20" s="14"/>
     </row>
-    <row r="21" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="12"/>
       <c r="C21" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B23)</f>
         <v>R8</v>
       </c>
-      <c r="D21" s="149">
+      <c r="D21" s="150">
         <f>Matriz!E23</f>
         <v>0</v>
       </c>
-      <c r="E21" s="149"/>
-      <c r="F21" s="58">
+      <c r="E21" s="150"/>
+      <c r="F21" s="57">
         <f>Matriz!F23</f>
         <v>0</v>
       </c>
-      <c r="G21" s="59"/>
-      <c r="H21" s="58">
+      <c r="G21" s="58"/>
+      <c r="H21" s="57">
         <f>Matriz!H23</f>
         <v>0</v>
       </c>
-      <c r="I21" s="58">
+      <c r="I21" s="57">
         <f>Matriz!I23</f>
         <v>0</v>
       </c>
-      <c r="J21" s="60">
+      <c r="J21" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K21" s="60" t="str">
+      <c r="K21" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="L21" s="61">
+      <c r="L21" s="60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M21" s="14"/>
     </row>
-    <row r="22" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="12"/>
       <c r="C22" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B24)</f>
         <v>R9</v>
       </c>
-      <c r="D22" s="149">
+      <c r="D22" s="150">
         <f>Matriz!E24</f>
         <v>0</v>
       </c>
-      <c r="E22" s="149"/>
-      <c r="F22" s="58">
+      <c r="E22" s="150"/>
+      <c r="F22" s="57">
         <f>Matriz!F24</f>
         <v>0</v>
       </c>
-      <c r="G22" s="59"/>
-      <c r="H22" s="58">
+      <c r="G22" s="58"/>
+      <c r="H22" s="57">
         <f>Matriz!H24</f>
         <v>0</v>
       </c>
-      <c r="I22" s="58">
+      <c r="I22" s="57">
         <f>Matriz!I24</f>
         <v>0</v>
       </c>
-      <c r="J22" s="60">
+      <c r="J22" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K22" s="60" t="str">
+      <c r="K22" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="L22" s="61">
+      <c r="L22" s="60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M22" s="14"/>
     </row>
-    <row r="23" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="12"/>
       <c r="C23" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B25)</f>
         <v>R10</v>
       </c>
-      <c r="D23" s="149">
+      <c r="D23" s="150">
         <f>Matriz!E25</f>
         <v>0</v>
       </c>
-      <c r="E23" s="149"/>
-      <c r="F23" s="58">
+      <c r="E23" s="150"/>
+      <c r="F23" s="57">
         <f>Matriz!F25</f>
         <v>0</v>
       </c>
-      <c r="G23" s="59"/>
-      <c r="H23" s="58">
+      <c r="G23" s="58"/>
+      <c r="H23" s="57">
         <f>Matriz!H25</f>
         <v>0</v>
       </c>
-      <c r="I23" s="58">
+      <c r="I23" s="57">
         <f>Matriz!I25</f>
         <v>0</v>
       </c>
-      <c r="J23" s="60">
+      <c r="J23" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K23" s="60" t="str">
+      <c r="K23" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="L23" s="61">
+      <c r="L23" s="60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M23" s="14"/>
     </row>
-    <row r="24" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="12"/>
       <c r="C24" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B26)</f>
         <v>R11</v>
       </c>
-      <c r="D24" s="149">
+      <c r="D24" s="150">
         <f>Matriz!E26</f>
         <v>0</v>
       </c>
-      <c r="E24" s="149"/>
-      <c r="F24" s="58">
+      <c r="E24" s="150"/>
+      <c r="F24" s="57">
         <f>Matriz!F26</f>
         <v>0</v>
       </c>
-      <c r="G24" s="59"/>
-      <c r="H24" s="58">
+      <c r="G24" s="58"/>
+      <c r="H24" s="57">
         <f>Matriz!H26</f>
         <v>0</v>
       </c>
-      <c r="I24" s="58">
+      <c r="I24" s="57">
         <f>Matriz!I26</f>
         <v>0</v>
       </c>
-      <c r="J24" s="60">
+      <c r="J24" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K24" s="60" t="str">
+      <c r="K24" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="L24" s="61">
+      <c r="L24" s="60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M24" s="14"/>
     </row>
-    <row r="25" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="12"/>
       <c r="C25" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B27)</f>
         <v>R12</v>
       </c>
-      <c r="D25" s="149">
+      <c r="D25" s="150">
         <f>Matriz!E27</f>
         <v>0</v>
       </c>
-      <c r="E25" s="149"/>
-      <c r="F25" s="58">
+      <c r="E25" s="150"/>
+      <c r="F25" s="57">
         <f>Matriz!F27</f>
         <v>0</v>
       </c>
-      <c r="G25" s="59"/>
-      <c r="H25" s="58">
+      <c r="G25" s="58"/>
+      <c r="H25" s="57">
         <f>Matriz!H27</f>
         <v>0</v>
       </c>
-      <c r="I25" s="58">
+      <c r="I25" s="57">
         <f>Matriz!I27</f>
         <v>0</v>
       </c>
-      <c r="J25" s="60">
+      <c r="J25" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K25" s="60" t="str">
+      <c r="K25" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="L25" s="61">
+      <c r="L25" s="60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M25" s="14"/>
     </row>
-    <row r="26" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="12"/>
       <c r="C26" s="53" t="str">
         <f>CONCATENATE($B$13,Matriz!B28)</f>
         <v>R13</v>
       </c>
-      <c r="D26" s="149">
+      <c r="D26" s="150">
         <f>Matriz!E28</f>
         <v>0</v>
       </c>
-      <c r="E26" s="149"/>
-      <c r="F26" s="58">
+      <c r="E26" s="150"/>
+      <c r="F26" s="57">
         <f>Matriz!F28</f>
         <v>0</v>
       </c>
-      <c r="G26" s="59"/>
-      <c r="H26" s="58">
+      <c r="G26" s="58"/>
+      <c r="H26" s="57">
         <f>Matriz!H28</f>
         <v>0</v>
       </c>
-      <c r="I26" s="58">
+      <c r="I26" s="57">
         <f>Matriz!I28</f>
         <v>0</v>
       </c>
-      <c r="J26" s="60">
+      <c r="J26" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K26" s="60" t="str">
+      <c r="K26" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="L26" s="61">
+      <c r="L26" s="60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M26" s="14"/>
     </row>
-    <row r="27" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="12"/>
       <c r="C27" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B29)</f>
         <v>R14</v>
       </c>
-      <c r="D27" s="149">
+      <c r="D27" s="150">
         <f>Matriz!E29</f>
         <v>0</v>
       </c>
-      <c r="E27" s="149"/>
-      <c r="F27" s="58">
+      <c r="E27" s="150"/>
+      <c r="F27" s="57">
         <f>Matriz!F29</f>
         <v>0</v>
       </c>
-      <c r="G27" s="59"/>
-      <c r="H27" s="58">
+      <c r="G27" s="58"/>
+      <c r="H27" s="57">
         <f>Matriz!H29</f>
         <v>0</v>
       </c>
-      <c r="I27" s="58">
+      <c r="I27" s="57">
         <f>Matriz!I29</f>
         <v>0</v>
       </c>
-      <c r="J27" s="60">
+      <c r="J27" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K27" s="60" t="str">
+      <c r="K27" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="L27" s="61">
+      <c r="L27" s="60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M27" s="14"/>
     </row>
-    <row r="28" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="12"/>
       <c r="C28" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B30)</f>
         <v>R15</v>
       </c>
-      <c r="D28" s="149">
+      <c r="D28" s="150">
         <f>Matriz!E30</f>
         <v>0</v>
       </c>
-      <c r="E28" s="149"/>
-      <c r="F28" s="58">
+      <c r="E28" s="150"/>
+      <c r="F28" s="57">
         <f>Matriz!F30</f>
         <v>0</v>
       </c>
-      <c r="G28" s="59"/>
-      <c r="H28" s="58">
+      <c r="G28" s="58"/>
+      <c r="H28" s="57">
         <f>Matriz!H30</f>
         <v>0</v>
       </c>
-      <c r="I28" s="58">
+      <c r="I28" s="57">
         <f>Matriz!I30</f>
         <v>0</v>
       </c>
-      <c r="J28" s="60">
+      <c r="J28" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K28" s="60" t="str">
+      <c r="K28" s="59" t="str">
         <f t="shared" si="1"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="L28" s="61">
+      <c r="L28" s="60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M28" s="14"/>
     </row>
-    <row r="29" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -3695,23 +3718,23 @@
       <c r="L29" s="13"/>
       <c r="M29" s="14"/>
     </row>
-    <row r="30" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="150" t="s">
+    <row r="30" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="151" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="150"/>
-      <c r="D30" s="150"/>
-      <c r="E30" s="150"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="150"/>
-      <c r="H30" s="150"/>
-      <c r="I30" s="150"/>
-      <c r="J30" s="150"/>
-      <c r="K30" s="150"/>
-      <c r="L30" s="150"/>
-      <c r="M30" s="150"/>
-    </row>
-    <row r="31" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="151"/>
+      <c r="D30" s="151"/>
+      <c r="E30" s="151"/>
+      <c r="F30" s="151"/>
+      <c r="G30" s="151"/>
+      <c r="H30" s="151"/>
+      <c r="I30" s="151"/>
+      <c r="J30" s="151"/>
+      <c r="K30" s="151"/>
+      <c r="L30" s="151"/>
+      <c r="M30" s="151"/>
+    </row>
+    <row r="31" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -3725,532 +3748,532 @@
       <c r="L31" s="13"/>
       <c r="M31" s="14"/>
     </row>
-    <row r="32" spans="2:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="12"/>
-      <c r="C32" s="62" t="s">
+      <c r="C32" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="151" t="s">
+      <c r="D32" s="152" t="s">
         <v>53</v>
       </c>
-      <c r="E32" s="151"/>
-      <c r="F32" s="63" t="s">
+      <c r="E32" s="152"/>
+      <c r="F32" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="63" t="s">
+      <c r="G32" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="H32" s="63" t="s">
+      <c r="H32" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="I32" s="63" t="s">
+      <c r="I32" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="J32" s="63" t="s">
+      <c r="J32" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="K32" s="152" t="s">
+      <c r="K32" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="L32" s="152"/>
+      <c r="L32" s="153"/>
       <c r="M32" s="14"/>
     </row>
-    <row r="33" spans="2:13" ht="163.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:13" ht="163.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="12"/>
-      <c r="C33" s="64" t="str">
+      <c r="C33" s="63" t="str">
         <f t="shared" ref="C33:D47" si="3">C14</f>
         <v>R1</v>
       </c>
-      <c r="D33" s="146" t="str">
+      <c r="D33" s="147" t="str">
         <f t="shared" si="3"/>
         <v>no trabajar eficientemente</v>
       </c>
-      <c r="E33" s="146"/>
-      <c r="F33" s="66" t="str">
+      <c r="E33" s="147"/>
+      <c r="F33" s="65" t="str">
         <f t="shared" ref="F33:F47" si="4">K14</f>
-        <v>MODERADO</v>
-      </c>
-      <c r="G33" s="65" t="s">
+        <v>ALTO</v>
+      </c>
+      <c r="G33" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="H33" s="65" t="str">
+      <c r="H33" s="64" t="str">
         <f>Matriz!K16</f>
         <v>•Realización de reuniones sobre avances del proyecto
 •Realizar acuerdos y trabajar en un punto medio de opiniones</v>
       </c>
-      <c r="I33" s="65" t="s">
+      <c r="I33" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J33" s="65" t="s">
-        <v>82</v>
-      </c>
-      <c r="K33" s="147" t="str">
+      <c r="J33" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="K33" s="148" t="str">
         <f>Matriz!K16</f>
         <v>•Realización de reuniones sobre avances del proyecto
 •Realizar acuerdos y trabajar en un punto medio de opiniones</v>
       </c>
-      <c r="L33" s="147"/>
+      <c r="L33" s="148"/>
       <c r="M33" s="14"/>
     </row>
-    <row r="34" spans="2:13" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="12"/>
-      <c r="C34" s="67" t="str">
+      <c r="C34" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R2</v>
       </c>
-      <c r="D34" s="148" t="str">
+      <c r="D34" s="149" t="str">
         <f t="shared" si="3"/>
         <v>Tiempos incongruentes y fechas mal planeadas ,Organización ineficiente</v>
       </c>
-      <c r="E34" s="148"/>
-      <c r="F34" s="68" t="str">
+      <c r="E34" s="149"/>
+      <c r="F34" s="67" t="str">
         <f t="shared" si="4"/>
         <v>MODERADO</v>
       </c>
-      <c r="G34" s="69" t="s">
+      <c r="G34" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="89" t="str">
+      <c r="H34" s="88" t="str">
         <f>Matriz!K17</f>
         <v>Revisar actividades con fechas y ajustarlos a tiempos del proyecto, utilizar un repositorio para el almacenamiento de la información.</v>
       </c>
-      <c r="I34" s="65" t="s">
+      <c r="I34" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J34" s="69" t="s">
-        <v>82</v>
-      </c>
-      <c r="K34" s="145" t="str">
+      <c r="J34" s="68" t="s">
+        <v>125</v>
+      </c>
+      <c r="K34" s="146" t="str">
         <f>Matriz!K17</f>
         <v>Revisar actividades con fechas y ajustarlos a tiempos del proyecto, utilizar un repositorio para el almacenamiento de la información.</v>
       </c>
-      <c r="L34" s="145"/>
+      <c r="L34" s="146"/>
       <c r="M34" s="14"/>
     </row>
-    <row r="35" spans="2:13" ht="125.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:13" ht="125.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="12"/>
-      <c r="C35" s="67" t="str">
+      <c r="C35" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R3</v>
       </c>
-      <c r="D35" s="144" t="str">
+      <c r="D35" s="145" t="str">
         <f t="shared" si="3"/>
         <v>Cambios regulares y nuevos añadidos a los requerimientos</v>
       </c>
-      <c r="E35" s="144"/>
-      <c r="F35" s="71" t="str">
+      <c r="E35" s="145"/>
+      <c r="F35" s="70" t="str">
         <f t="shared" si="4"/>
         <v>MODERADO</v>
       </c>
-      <c r="G35" s="70" t="s">
+      <c r="G35" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="89" t="str">
+      <c r="H35" s="88" t="str">
         <f>Matriz!K18</f>
-        <v xml:space="preserve">Acoplar los requerimientos nuevos cambios o existentes de forma clara y  eficiente  para cumplir la funcionalidad planeada </v>
-      </c>
-      <c r="I35" s="65" t="s">
+        <v xml:space="preserve">Acoplar los requerimientos nuevos o cambios  existentes de forma clara y  eficiente  para cumplir la funcionalidad planeada </v>
+      </c>
+      <c r="I35" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J35" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="K35" s="145" t="str">
+      <c r="J35" s="69" t="s">
+        <v>125</v>
+      </c>
+      <c r="K35" s="146" t="str">
         <f>Matriz!K18</f>
-        <v xml:space="preserve">Acoplar los requerimientos nuevos cambios o existentes de forma clara y  eficiente  para cumplir la funcionalidad planeada </v>
-      </c>
-      <c r="L35" s="145"/>
+        <v xml:space="preserve">Acoplar los requerimientos nuevos o cambios  existentes de forma clara y  eficiente  para cumplir la funcionalidad planeada </v>
+      </c>
+      <c r="L35" s="146"/>
       <c r="M35" s="14"/>
     </row>
-    <row r="36" spans="2:13" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:13" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="12"/>
-      <c r="C36" s="67" t="str">
+      <c r="C36" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R4</v>
       </c>
-      <c r="D36" s="144" t="str">
+      <c r="D36" s="145" t="str">
         <f t="shared" si="3"/>
         <v>interpretación erronea de las ventanas e interfaces</v>
       </c>
-      <c r="E36" s="144"/>
-      <c r="F36" s="68" t="str">
+      <c r="E36" s="145"/>
+      <c r="F36" s="67" t="str">
         <f t="shared" si="4"/>
         <v>BAJO</v>
       </c>
-      <c r="G36" s="69" t="s">
+      <c r="G36" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="H36" s="89" t="str">
+      <c r="H36" s="88" t="str">
         <f>Matriz!K19</f>
         <v>Rediseñar las interfaces con base  a los requerimientos de software</v>
       </c>
-      <c r="I36" s="65" t="s">
+      <c r="I36" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J36" s="69" t="s">
+      <c r="J36" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="K36" s="145" t="str">
+      <c r="K36" s="146" t="str">
         <f>Matriz!K19</f>
         <v>Rediseñar las interfaces con base  a los requerimientos de software</v>
       </c>
-      <c r="L36" s="145"/>
+      <c r="L36" s="146"/>
       <c r="M36" s="14"/>
     </row>
-    <row r="37" spans="2:13" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:13" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="12"/>
-      <c r="C37" s="67" t="str">
+      <c r="C37" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R5</v>
       </c>
-      <c r="D37" s="144" t="str">
+      <c r="D37" s="145" t="str">
         <f t="shared" si="3"/>
         <v>Estructuración erronea de los datos, tablas mal relacionadas</v>
       </c>
-      <c r="E37" s="144"/>
-      <c r="F37" s="71" t="str">
+      <c r="E37" s="145"/>
+      <c r="F37" s="70" t="str">
         <f t="shared" si="4"/>
         <v>MODERADO</v>
       </c>
-      <c r="G37" s="70" t="s">
+      <c r="G37" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="H37" s="89" t="str">
+      <c r="H37" s="88" t="str">
         <f>Matriz!K20</f>
         <v>Redefinir la arquitectura lógica llevando a cabo un analisis produndo para lograr  relaciones de tablas correctas con base a los procesos de la empresa</v>
       </c>
-      <c r="I37" s="65" t="s">
+      <c r="I37" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J37" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="K37" s="145" t="str">
+      <c r="J37" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="K37" s="146" t="str">
         <f>Matriz!K20</f>
         <v>Redefinir la arquitectura lógica llevando a cabo un analisis produndo para lograr  relaciones de tablas correctas con base a los procesos de la empresa</v>
       </c>
-      <c r="L37" s="145"/>
+      <c r="L37" s="146"/>
       <c r="M37" s="14"/>
     </row>
-    <row r="38" spans="2:13" ht="194.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" ht="194.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="12"/>
-      <c r="C38" s="72" t="str">
+      <c r="C38" s="71" t="str">
         <f t="shared" si="3"/>
         <v>R6</v>
       </c>
-      <c r="D38" s="142" t="str">
+      <c r="D38" s="143" t="str">
         <f t="shared" si="3"/>
         <v>Pruebas ineficientes</v>
       </c>
-      <c r="E38" s="142"/>
-      <c r="F38" s="73" t="str">
+      <c r="E38" s="143"/>
+      <c r="F38" s="72" t="str">
         <f t="shared" si="4"/>
         <v>ALTO</v>
       </c>
-      <c r="G38" s="74" t="s">
-        <v>101</v>
-      </c>
-      <c r="H38" s="89" t="str">
+      <c r="G38" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="H38" s="88" t="str">
         <f>Matriz!K21</f>
         <v>•Realizar pruebas completas sobre cada módulo de la aplicación asegurandose de cumplir la funcionalidad principal
 •Darle seguimiento a cada falla encontrado
 •someter nuevamente a pruebas los módulos donde se reportaron fallas</v>
       </c>
-      <c r="I38" s="65" t="s">
+      <c r="I38" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J38" s="74" t="s">
-        <v>101</v>
-      </c>
-      <c r="K38" s="143" t="str">
+      <c r="J38" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="K38" s="144" t="str">
         <f>Matriz!K21</f>
         <v>•Realizar pruebas completas sobre cada módulo de la aplicación asegurandose de cumplir la funcionalidad principal
 •Darle seguimiento a cada falla encontrado
 •someter nuevamente a pruebas los módulos donde se reportaron fallas</v>
       </c>
-      <c r="L38" s="143"/>
+      <c r="L38" s="144"/>
       <c r="M38" s="14"/>
     </row>
-    <row r="39" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="12"/>
-      <c r="C39" s="67" t="str">
+      <c r="C39" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R7</v>
       </c>
-      <c r="D39" s="142">
+      <c r="D39" s="143">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E39" s="142"/>
-      <c r="F39" s="73" t="str">
+      <c r="E39" s="143"/>
+      <c r="F39" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="G39" s="74"/>
-      <c r="H39" s="89">
+      <c r="G39" s="73"/>
+      <c r="H39" s="88">
         <f>Matriz!K22</f>
         <v>0</v>
       </c>
-      <c r="I39" s="65" t="s">
+      <c r="I39" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J39" s="74"/>
-      <c r="K39" s="143">
+      <c r="J39" s="73"/>
+      <c r="K39" s="144">
         <f>Matriz!K22</f>
         <v>0</v>
       </c>
-      <c r="L39" s="143"/>
+      <c r="L39" s="144"/>
       <c r="M39" s="14"/>
     </row>
-    <row r="40" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="12"/>
-      <c r="C40" s="67" t="str">
+      <c r="C40" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R8</v>
       </c>
-      <c r="D40" s="142">
+      <c r="D40" s="143">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E40" s="142"/>
-      <c r="F40" s="73" t="str">
+      <c r="E40" s="143"/>
+      <c r="F40" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="G40" s="74"/>
-      <c r="H40" s="89">
+      <c r="G40" s="73"/>
+      <c r="H40" s="88">
         <f>Matriz!K23</f>
         <v>0</v>
       </c>
-      <c r="I40" s="65" t="s">
+      <c r="I40" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J40" s="74"/>
-      <c r="K40" s="143">
+      <c r="J40" s="73"/>
+      <c r="K40" s="144">
         <f>Matriz!K23</f>
         <v>0</v>
       </c>
-      <c r="L40" s="143"/>
+      <c r="L40" s="144"/>
       <c r="M40" s="14"/>
     </row>
-    <row r="41" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="12"/>
-      <c r="C41" s="67" t="str">
+      <c r="C41" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R9</v>
       </c>
-      <c r="D41" s="142">
+      <c r="D41" s="143">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E41" s="142"/>
-      <c r="F41" s="73" t="str">
+      <c r="E41" s="143"/>
+      <c r="F41" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="G41" s="74"/>
-      <c r="H41" s="89">
+      <c r="G41" s="73"/>
+      <c r="H41" s="88">
         <f>Matriz!K24</f>
         <v>0</v>
       </c>
-      <c r="I41" s="65" t="s">
+      <c r="I41" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J41" s="74"/>
-      <c r="K41" s="143">
+      <c r="J41" s="73"/>
+      <c r="K41" s="144">
         <f>Matriz!K24</f>
         <v>0</v>
       </c>
-      <c r="L41" s="143"/>
+      <c r="L41" s="144"/>
       <c r="M41" s="14"/>
     </row>
-    <row r="42" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="12"/>
-      <c r="C42" s="67" t="str">
+      <c r="C42" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R10</v>
       </c>
-      <c r="D42" s="142">
+      <c r="D42" s="143">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E42" s="142"/>
-      <c r="F42" s="73" t="str">
+      <c r="E42" s="143"/>
+      <c r="F42" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="G42" s="74"/>
-      <c r="H42" s="89">
+      <c r="G42" s="73"/>
+      <c r="H42" s="88">
         <f>Matriz!K25</f>
         <v>0</v>
       </c>
-      <c r="I42" s="65" t="s">
+      <c r="I42" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J42" s="74"/>
-      <c r="K42" s="143">
+      <c r="J42" s="73"/>
+      <c r="K42" s="144">
         <f>Matriz!K25</f>
         <v>0</v>
       </c>
-      <c r="L42" s="143"/>
+      <c r="L42" s="144"/>
       <c r="M42" s="14"/>
     </row>
-    <row r="43" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="12"/>
-      <c r="C43" s="72" t="str">
+      <c r="C43" s="71" t="str">
         <f t="shared" si="3"/>
         <v>R11</v>
       </c>
-      <c r="D43" s="142">
+      <c r="D43" s="143">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E43" s="142"/>
-      <c r="F43" s="73" t="str">
+      <c r="E43" s="143"/>
+      <c r="F43" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="G43" s="74"/>
-      <c r="H43" s="89">
+      <c r="G43" s="73"/>
+      <c r="H43" s="88">
         <f>Matriz!K26</f>
         <v>0</v>
       </c>
-      <c r="I43" s="65" t="s">
+      <c r="I43" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J43" s="74"/>
-      <c r="K43" s="143">
+      <c r="J43" s="73"/>
+      <c r="K43" s="144">
         <f>Matriz!K26</f>
         <v>0</v>
       </c>
-      <c r="L43" s="143"/>
+      <c r="L43" s="144"/>
       <c r="M43" s="14"/>
     </row>
-    <row r="44" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="12"/>
-      <c r="C44" s="67" t="str">
+      <c r="C44" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R12</v>
       </c>
-      <c r="D44" s="142">
+      <c r="D44" s="143">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E44" s="142"/>
-      <c r="F44" s="73" t="str">
+      <c r="E44" s="143"/>
+      <c r="F44" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="G44" s="74"/>
-      <c r="H44" s="89">
+      <c r="G44" s="73"/>
+      <c r="H44" s="88">
         <f>Matriz!K27</f>
         <v>0</v>
       </c>
-      <c r="I44" s="65" t="s">
+      <c r="I44" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J44" s="74"/>
-      <c r="K44" s="143">
+      <c r="J44" s="73"/>
+      <c r="K44" s="144">
         <f>Matriz!K27</f>
         <v>0</v>
       </c>
-      <c r="L44" s="143"/>
+      <c r="L44" s="144"/>
       <c r="M44" s="14"/>
     </row>
-    <row r="45" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="12"/>
-      <c r="C45" s="67" t="str">
+      <c r="C45" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R13</v>
       </c>
-      <c r="D45" s="142">
+      <c r="D45" s="143">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E45" s="142"/>
-      <c r="F45" s="73" t="str">
+      <c r="E45" s="143"/>
+      <c r="F45" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="G45" s="74"/>
-      <c r="H45" s="89">
+      <c r="G45" s="73"/>
+      <c r="H45" s="88">
         <f>Matriz!K28</f>
         <v>0</v>
       </c>
-      <c r="I45" s="65" t="s">
+      <c r="I45" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J45" s="74"/>
-      <c r="K45" s="143">
+      <c r="J45" s="73"/>
+      <c r="K45" s="144">
         <f>Matriz!K28</f>
         <v>0</v>
       </c>
-      <c r="L45" s="143"/>
+      <c r="L45" s="144"/>
       <c r="M45" s="14"/>
     </row>
-    <row r="46" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="12"/>
-      <c r="C46" s="67" t="str">
+      <c r="C46" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R14</v>
       </c>
-      <c r="D46" s="142">
+      <c r="D46" s="143">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E46" s="142"/>
-      <c r="F46" s="73" t="str">
+      <c r="E46" s="143"/>
+      <c r="F46" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="G46" s="74"/>
-      <c r="H46" s="89">
+      <c r="G46" s="73"/>
+      <c r="H46" s="88">
         <f>Matriz!K29</f>
         <v>0</v>
       </c>
-      <c r="I46" s="65" t="s">
+      <c r="I46" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J46" s="74"/>
-      <c r="K46" s="143">
+      <c r="J46" s="73"/>
+      <c r="K46" s="144">
         <f>Matriz!K29</f>
         <v>0</v>
       </c>
-      <c r="L46" s="143"/>
+      <c r="L46" s="144"/>
       <c r="M46" s="14"/>
     </row>
-    <row r="47" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
-      <c r="C47" s="67" t="str">
+      <c r="C47" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R15</v>
       </c>
-      <c r="D47" s="142">
+      <c r="D47" s="143">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E47" s="142"/>
-      <c r="F47" s="73" t="str">
+      <c r="E47" s="143"/>
+      <c r="F47" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
       </c>
-      <c r="G47" s="74"/>
-      <c r="H47" s="89">
+      <c r="G47" s="73"/>
+      <c r="H47" s="88">
         <f>Matriz!K30</f>
         <v>0</v>
       </c>
-      <c r="I47" s="65" t="s">
+      <c r="I47" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="J47" s="74"/>
-      <c r="K47" s="143">
+      <c r="J47" s="73"/>
+      <c r="K47" s="144">
         <f>Matriz!K30</f>
         <v>0</v>
       </c>
-      <c r="L47" s="143"/>
+      <c r="L47" s="144"/>
       <c r="M47" s="14"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B48" s="12"/>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
@@ -4264,7 +4287,7 @@
       <c r="L48" s="13"/>
       <c r="M48" s="14"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B49" s="12"/>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
@@ -4278,19 +4301,19 @@
       <c r="L49" s="13"/>
       <c r="M49" s="14"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B50" s="75"/>
-      <c r="C50" s="76"/>
-      <c r="D50" s="76"/>
-      <c r="E50" s="76"/>
-      <c r="F50" s="76"/>
-      <c r="G50" s="76"/>
-      <c r="H50" s="76"/>
-      <c r="I50" s="76"/>
-      <c r="J50" s="76"/>
-      <c r="K50" s="76"/>
-      <c r="L50" s="76"/>
-      <c r="M50" s="77"/>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B50" s="74"/>
+      <c r="C50" s="75"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="75"/>
+      <c r="F50" s="75"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="75"/>
+      <c r="I50" s="75"/>
+      <c r="J50" s="75"/>
+      <c r="K50" s="75"/>
+      <c r="L50" s="75"/>
+      <c r="M50" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="56">
@@ -4403,39 +4426,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13:N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="11.5546875"/>
-    <col min="8" max="8" width="18.88671875" customWidth="1"/>
+    <col min="1" max="7" width="11.5703125"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="11" width="11.5546875"/>
-    <col min="12" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="1025" width="11.5546875"/>
+    <col min="10" max="11" width="11.5703125"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="3:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="161" t="s">
+    <row r="4" spans="3:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="162" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="161"/>
-      <c r="E5" s="161"/>
-      <c r="F5" s="161"/>
-      <c r="G5" s="161"/>
-      <c r="H5" s="161"/>
-      <c r="I5" s="161"/>
-      <c r="J5" s="161"/>
-      <c r="K5" s="161"/>
-      <c r="L5" s="161"/>
-      <c r="M5" s="161"/>
-      <c r="N5" s="161"/>
-      <c r="O5" s="161"/>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="162"/>
+      <c r="H5" s="162"/>
+      <c r="I5" s="162"/>
+      <c r="J5" s="162"/>
+      <c r="K5" s="162"/>
+      <c r="L5" s="162"/>
+      <c r="M5" s="162"/>
+      <c r="N5" s="162"/>
+      <c r="O5" s="162"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -4450,564 +4473,567 @@
       <c r="N6" s="13"/>
       <c r="O6" s="14"/>
     </row>
-    <row r="7" spans="3:15" ht="33.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:15" ht="33.200000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="12"/>
-      <c r="D7" s="78" t="s">
+      <c r="D7" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="162" t="s">
+      <c r="E7" s="163" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="162"/>
-      <c r="G7" s="78" t="s">
+      <c r="F7" s="163"/>
+      <c r="G7" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="78" t="s">
+      <c r="H7" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="I7" s="78" t="s">
+      <c r="I7" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="J7" s="78" t="s">
+      <c r="J7" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="78" t="s">
+      <c r="K7" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="78" t="s">
+      <c r="L7" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="162" t="s">
+      <c r="M7" s="163" t="s">
         <v>73</v>
       </c>
-      <c r="N7" s="162"/>
+      <c r="N7" s="163"/>
       <c r="O7" s="14"/>
     </row>
-    <row r="8" spans="3:15" ht="146.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:15" ht="146.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="12"/>
-      <c r="D8" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C33</f>
+      <c r="D8" s="78" t="str">
+        <f>'Cualitativo '!C33</f>
         <v>R1</v>
       </c>
-      <c r="E8" s="160" t="str">
-        <f>'Cualitativo y Cuantitativo'!D33</f>
+      <c r="E8" s="161" t="str">
+        <f>'Cualitativo '!D33</f>
         <v>no trabajar eficientemente</v>
       </c>
-      <c r="F8" s="160"/>
-      <c r="G8" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F33</f>
-        <v>MODERADO</v>
-      </c>
-      <c r="H8" s="80" t="str">
-        <f>'Cualitativo y Cuantitativo'!J33</f>
-        <v>Project Manager</v>
-      </c>
-      <c r="I8" s="80" t="str">
+      <c r="F8" s="161"/>
+      <c r="G8" s="80" t="str">
+        <f>'Cualitativo '!F33</f>
+        <v>ALTO</v>
+      </c>
+      <c r="H8" s="79" t="str">
+        <f>'Cualitativo '!J33</f>
+        <v>Portafolio manager</v>
+      </c>
+      <c r="I8" s="79" t="str">
         <f>Matriz!K16</f>
         <v>•Realización de reuniones sobre avances del proyecto
 •Realizar acuerdos y trabajar en un punto medio de opiniones</v>
       </c>
-      <c r="J8" s="82" t="s">
+      <c r="J8" s="167" t="s">
         <v>74</v>
       </c>
-      <c r="K8" s="106">
+      <c r="K8" s="105">
         <v>43565</v>
       </c>
-      <c r="L8" s="80" t="str">
-        <f>'Cualitativo y Cuantitativo'!J33</f>
-        <v>Project Manager</v>
-      </c>
-      <c r="M8" s="160" t="s">
-        <v>94</v>
-      </c>
-      <c r="N8" s="160"/>
+      <c r="L8" s="79" t="str">
+        <f>'Cualitativo '!J33</f>
+        <v>Portafolio manager</v>
+      </c>
+      <c r="M8" s="161" t="s">
+        <v>126</v>
+      </c>
+      <c r="N8" s="161"/>
       <c r="O8" s="14"/>
     </row>
-    <row r="9" spans="3:15" ht="113.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:15" ht="113.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="12"/>
-      <c r="D9" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C34</f>
+      <c r="D9" s="78" t="str">
+        <f>'Cualitativo '!C34</f>
         <v>R2</v>
       </c>
-      <c r="E9" s="160" t="str">
-        <f>'Cualitativo y Cuantitativo'!D34</f>
+      <c r="E9" s="161" t="str">
+        <f>'Cualitativo '!D34</f>
         <v>Tiempos incongruentes y fechas mal planeadas ,Organización ineficiente</v>
       </c>
-      <c r="F9" s="160"/>
-      <c r="G9" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F34</f>
+      <c r="F9" s="161"/>
+      <c r="G9" s="80" t="str">
+        <f>'Cualitativo '!F34</f>
         <v>MODERADO</v>
       </c>
-      <c r="H9" s="80" t="str">
-        <f>'Cualitativo y Cuantitativo'!J34</f>
-        <v>Project Manager</v>
-      </c>
-      <c r="I9" s="80" t="str">
+      <c r="H9" s="133" t="str">
+        <f>'Cualitativo '!J34</f>
+        <v>Portafolio manager</v>
+      </c>
+      <c r="I9" s="79" t="str">
         <f>Matriz!K17</f>
         <v>Revisar actividades con fechas y ajustarlos a tiempos del proyecto, utilizar un repositorio para el almacenamiento de la información.</v>
       </c>
-      <c r="J9" s="82" t="s">
+      <c r="J9" s="167" t="s">
         <v>74</v>
       </c>
-      <c r="K9" s="106">
+      <c r="K9" s="105">
         <v>43622</v>
       </c>
-      <c r="L9" s="80" t="str">
-        <f>'Cualitativo y Cuantitativo'!J34</f>
-        <v>Project Manager</v>
-      </c>
-      <c r="M9" s="160" t="s">
-        <v>103</v>
-      </c>
-      <c r="N9" s="160"/>
+      <c r="L9" s="79" t="str">
+        <f>'Cualitativo '!J34</f>
+        <v>Portafolio manager</v>
+      </c>
+      <c r="M9" s="161" t="s">
+        <v>129</v>
+      </c>
+      <c r="N9" s="161"/>
       <c r="O9" s="14"/>
     </row>
-    <row r="10" spans="3:15" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:15" ht="114.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="12"/>
-      <c r="D10" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C35</f>
+      <c r="D10" s="78" t="str">
+        <f>'Cualitativo '!C35</f>
         <v>R3</v>
       </c>
-      <c r="E10" s="160" t="str">
-        <f>'Cualitativo y Cuantitativo'!D35</f>
+      <c r="E10" s="161" t="str">
+        <f>'Cualitativo '!D35</f>
         <v>Cambios regulares y nuevos añadidos a los requerimientos</v>
       </c>
-      <c r="F10" s="160"/>
-      <c r="G10" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F35</f>
+      <c r="F10" s="161"/>
+      <c r="G10" s="80" t="str">
+        <f>'Cualitativo '!F35</f>
         <v>MODERADO</v>
       </c>
-      <c r="H10" s="80" t="str">
-        <f>'Cualitativo y Cuantitativo'!J35</f>
-        <v>Project Manager</v>
-      </c>
-      <c r="I10" s="108" t="str">
+      <c r="H10" s="133" t="str">
+        <f>'Cualitativo '!J35</f>
+        <v>Portafolio manager</v>
+      </c>
+      <c r="I10" s="107" t="str">
         <f>Matriz!K18</f>
-        <v xml:space="preserve">Acoplar los requerimientos nuevos cambios o existentes de forma clara y  eficiente  para cumplir la funcionalidad planeada </v>
-      </c>
-      <c r="J10" s="82" t="s">
+        <v xml:space="preserve">Acoplar los requerimientos nuevos o cambios  existentes de forma clara y  eficiente  para cumplir la funcionalidad planeada </v>
+      </c>
+      <c r="J10" s="167" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="106">
+      <c r="K10" s="105">
         <v>43631</v>
       </c>
-      <c r="L10" s="80" t="str">
-        <f>'Cualitativo y Cuantitativo'!J35</f>
-        <v>Project Manager</v>
-      </c>
-      <c r="M10" s="160" t="s">
-        <v>102</v>
-      </c>
-      <c r="N10" s="160"/>
+      <c r="L10" s="79" t="str">
+        <f>'Cualitativo '!J35</f>
+        <v>Portafolio manager</v>
+      </c>
+      <c r="M10" s="161" t="s">
+        <v>130</v>
+      </c>
+      <c r="N10" s="161"/>
       <c r="O10" s="14"/>
     </row>
-    <row r="11" spans="3:15" ht="92.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:15" ht="92.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="12"/>
-      <c r="D11" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C36</f>
+      <c r="D11" s="78" t="str">
+        <f>'Cualitativo '!C36</f>
         <v>R4</v>
       </c>
-      <c r="E11" s="160" t="str">
-        <f>'Cualitativo y Cuantitativo'!D36</f>
+      <c r="E11" s="161" t="str">
+        <f>'Cualitativo '!D36</f>
         <v>interpretación erronea de las ventanas e interfaces</v>
       </c>
-      <c r="F11" s="160"/>
-      <c r="G11" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F36</f>
+      <c r="F11" s="161"/>
+      <c r="G11" s="80" t="str">
+        <f>'Cualitativo '!F36</f>
         <v>BAJO</v>
       </c>
-      <c r="H11" s="80" t="s">
-        <v>89</v>
-      </c>
-      <c r="I11" s="80" t="str">
+      <c r="H11" s="133" t="str">
+        <f>'Cualitativo '!J36</f>
+        <v>Analista</v>
+      </c>
+      <c r="I11" s="79" t="str">
         <f>Matriz!K19</f>
         <v>Rediseñar las interfaces con base  a los requerimientos de software</v>
       </c>
-      <c r="J11" s="82" t="s">
+      <c r="J11" s="167" t="s">
         <v>74</v>
       </c>
-      <c r="K11" s="106">
+      <c r="K11" s="105">
         <v>43642</v>
       </c>
-      <c r="L11" s="80" t="s">
+      <c r="L11" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="M11" s="160"/>
-      <c r="N11" s="160"/>
+      <c r="M11" s="161" t="s">
+        <v>131</v>
+      </c>
+      <c r="N11" s="161"/>
       <c r="O11" s="14"/>
     </row>
-    <row r="12" spans="3:15" ht="137.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:15" ht="137.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="12"/>
-      <c r="D12" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C37</f>
+      <c r="D12" s="78" t="str">
+        <f>'Cualitativo '!C37</f>
         <v>R5</v>
       </c>
-      <c r="E12" s="160" t="str">
-        <f>'Cualitativo y Cuantitativo'!D37</f>
+      <c r="E12" s="161" t="str">
+        <f>'Cualitativo '!D37</f>
         <v>Estructuración erronea de los datos, tablas mal relacionadas</v>
       </c>
-      <c r="F12" s="160"/>
-      <c r="G12" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F37</f>
+      <c r="F12" s="161"/>
+      <c r="G12" s="80" t="str">
+        <f>'Cualitativo '!F37</f>
         <v>MODERADO</v>
       </c>
-      <c r="H12" s="80" t="str">
-        <f>'Cualitativo y Cuantitativo'!J37</f>
-        <v>Project Manager</v>
-      </c>
-      <c r="I12" s="80" t="str">
+      <c r="H12" s="133" t="str">
+        <f>'Cualitativo '!J37</f>
+        <v>Analista</v>
+      </c>
+      <c r="I12" s="79" t="str">
         <f>Matriz!K20</f>
         <v>Redefinir la arquitectura lógica llevando a cabo un analisis produndo para lograr  relaciones de tablas correctas con base a los procesos de la empresa</v>
       </c>
-      <c r="J12" s="82" t="s">
+      <c r="J12" s="167" t="s">
         <v>74</v>
       </c>
-      <c r="K12" s="106">
+      <c r="K12" s="105">
         <v>43645</v>
       </c>
-      <c r="L12" s="80" t="str">
-        <f>'Cualitativo y Cuantitativo'!J37</f>
-        <v>Project Manager</v>
-      </c>
-      <c r="M12" s="160" t="s">
-        <v>104</v>
-      </c>
-      <c r="N12" s="160"/>
+      <c r="L12" s="79" t="str">
+        <f>'Cualitativo '!J37</f>
+        <v>Analista</v>
+      </c>
+      <c r="M12" s="161" t="s">
+        <v>132</v>
+      </c>
+      <c r="N12" s="161"/>
       <c r="O12" s="14"/>
     </row>
-    <row r="13" spans="3:15" ht="212.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:15" ht="212.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="12"/>
-      <c r="D13" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C38</f>
+      <c r="D13" s="78" t="str">
+        <f>'Cualitativo '!C38</f>
         <v>R6</v>
       </c>
-      <c r="E13" s="160" t="str">
-        <f>'Cualitativo y Cuantitativo'!D38</f>
+      <c r="E13" s="161" t="str">
+        <f>'Cualitativo '!D38</f>
         <v>Pruebas ineficientes</v>
       </c>
-      <c r="F13" s="160"/>
-      <c r="G13" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F38</f>
+      <c r="F13" s="161"/>
+      <c r="G13" s="80" t="str">
+        <f>'Cualitativo '!F38</f>
         <v>ALTO</v>
       </c>
-      <c r="H13" s="80" t="str">
-        <f>'Cualitativo y Cuantitativo'!J38</f>
-        <v>Análista</v>
-      </c>
-      <c r="I13" s="80" t="str">
+      <c r="H13" s="133" t="str">
+        <f>'Cualitativo '!J38</f>
+        <v>programador</v>
+      </c>
+      <c r="I13" s="79" t="str">
         <f>Matriz!K21</f>
         <v>•Realizar pruebas completas sobre cada módulo de la aplicación asegurandose de cumplir la funcionalidad principal
 •Darle seguimiento a cada falla encontrado
 •someter nuevamente a pruebas los módulos donde se reportaron fallas</v>
       </c>
-      <c r="J13" s="82"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="80" t="str">
-        <f>'Cualitativo y Cuantitativo'!J38</f>
-        <v>Análista</v>
-      </c>
-      <c r="M13" s="160"/>
-      <c r="N13" s="160"/>
+      <c r="J13" s="167"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="79" t="str">
+        <f>'Cualitativo '!J38</f>
+        <v>programador</v>
+      </c>
+      <c r="M13" s="161"/>
+      <c r="N13" s="161"/>
       <c r="O13" s="14"/>
     </row>
-    <row r="14" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="12"/>
-      <c r="D14" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C39</f>
+      <c r="D14" s="78" t="str">
+        <f>'Cualitativo '!C39</f>
         <v>R7</v>
       </c>
-      <c r="E14" s="160">
-        <f>'Cualitativo y Cuantitativo'!D39</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="160"/>
-      <c r="G14" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F39</f>
+      <c r="E14" s="161">
+        <f>'Cualitativo '!D39</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="161"/>
+      <c r="G14" s="80" t="str">
+        <f>'Cualitativo '!F39</f>
         <v>MUY BAJO</v>
       </c>
-      <c r="H14" s="80">
-        <f>'Cualitativo y Cuantitativo'!J39</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="80">
+      <c r="H14" s="79">
+        <f>'Cualitativo '!J39</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="79">
         <f>Matriz!K22</f>
         <v>0</v>
       </c>
-      <c r="J14" s="82"/>
-      <c r="K14" s="80"/>
-      <c r="L14" s="80">
-        <f>'Cualitativo y Cuantitativo'!J39</f>
-        <v>0</v>
-      </c>
-      <c r="M14" s="160"/>
-      <c r="N14" s="160"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="79">
+        <f>'Cualitativo '!J39</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="161"/>
+      <c r="N14" s="161"/>
       <c r="O14" s="14"/>
     </row>
-    <row r="15" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="12"/>
-      <c r="D15" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C40</f>
+      <c r="D15" s="78" t="str">
+        <f>'Cualitativo '!C40</f>
         <v>R8</v>
       </c>
-      <c r="E15" s="160">
-        <f>'Cualitativo y Cuantitativo'!D40</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="160"/>
-      <c r="G15" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F40</f>
+      <c r="E15" s="161">
+        <f>'Cualitativo '!D40</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="161"/>
+      <c r="G15" s="80" t="str">
+        <f>'Cualitativo '!F40</f>
         <v>MUY BAJO</v>
       </c>
-      <c r="H15" s="80">
-        <f>'Cualitativo y Cuantitativo'!J40</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="80">
+      <c r="H15" s="79">
+        <f>'Cualitativo '!J40</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="79">
         <f>Matriz!K23</f>
         <v>0</v>
       </c>
-      <c r="J15" s="82"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="80">
-        <f>'Cualitativo y Cuantitativo'!J40</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="160"/>
-      <c r="N15" s="160"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79">
+        <f>'Cualitativo '!J40</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="161"/>
+      <c r="N15" s="161"/>
       <c r="O15" s="14"/>
     </row>
-    <row r="16" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="12"/>
-      <c r="D16" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C41</f>
+      <c r="D16" s="78" t="str">
+        <f>'Cualitativo '!C41</f>
         <v>R9</v>
       </c>
-      <c r="E16" s="160">
-        <f>'Cualitativo y Cuantitativo'!D41</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="160"/>
-      <c r="G16" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F41</f>
+      <c r="E16" s="161">
+        <f>'Cualitativo '!D41</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="161"/>
+      <c r="G16" s="80" t="str">
+        <f>'Cualitativo '!F41</f>
         <v>MUY BAJO</v>
       </c>
-      <c r="H16" s="80">
-        <f>'Cualitativo y Cuantitativo'!J41</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="80">
+      <c r="H16" s="79">
+        <f>'Cualitativo '!J41</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="79">
         <f>Matriz!K24</f>
         <v>0</v>
       </c>
-      <c r="J16" s="82"/>
-      <c r="K16" s="80"/>
-      <c r="L16" s="80">
-        <f>'Cualitativo y Cuantitativo'!J41</f>
-        <v>0</v>
-      </c>
-      <c r="M16" s="160"/>
-      <c r="N16" s="160"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="79">
+        <f>'Cualitativo '!J41</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="161"/>
+      <c r="N16" s="161"/>
       <c r="O16" s="14"/>
     </row>
-    <row r="17" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="12"/>
-      <c r="D17" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C42</f>
+      <c r="D17" s="78" t="str">
+        <f>'Cualitativo '!C42</f>
         <v>R10</v>
       </c>
-      <c r="E17" s="160">
-        <f>'Cualitativo y Cuantitativo'!D42</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="160"/>
-      <c r="G17" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F42</f>
+      <c r="E17" s="161">
+        <f>'Cualitativo '!D42</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="161"/>
+      <c r="G17" s="80" t="str">
+        <f>'Cualitativo '!F42</f>
         <v>MUY BAJO</v>
       </c>
-      <c r="H17" s="80">
-        <f>'Cualitativo y Cuantitativo'!J42</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="80">
+      <c r="H17" s="79">
+        <f>'Cualitativo '!J42</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="79">
         <f>Matriz!K25</f>
         <v>0</v>
       </c>
-      <c r="J17" s="82"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="80">
-        <f>'Cualitativo y Cuantitativo'!J42</f>
-        <v>0</v>
-      </c>
-      <c r="M17" s="160"/>
-      <c r="N17" s="160"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="79">
+        <f>'Cualitativo '!J42</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="161"/>
+      <c r="N17" s="161"/>
       <c r="O17" s="14"/>
     </row>
-    <row r="18" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="12"/>
-      <c r="D18" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C43</f>
+      <c r="D18" s="78" t="str">
+        <f>'Cualitativo '!C43</f>
         <v>R11</v>
       </c>
-      <c r="E18" s="160">
-        <f>'Cualitativo y Cuantitativo'!D43</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="160"/>
-      <c r="G18" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F43</f>
+      <c r="E18" s="161">
+        <f>'Cualitativo '!D43</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="161"/>
+      <c r="G18" s="80" t="str">
+        <f>'Cualitativo '!F43</f>
         <v>MUY BAJO</v>
       </c>
-      <c r="H18" s="80">
-        <f>'Cualitativo y Cuantitativo'!J43</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="80">
+      <c r="H18" s="79">
+        <f>'Cualitativo '!J43</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="79">
         <f>Matriz!K26</f>
         <v>0</v>
       </c>
-      <c r="J18" s="82"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80">
-        <f>'Cualitativo y Cuantitativo'!J43</f>
-        <v>0</v>
-      </c>
-      <c r="M18" s="160"/>
-      <c r="N18" s="160"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="79">
+        <f>'Cualitativo '!J43</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="161"/>
+      <c r="N18" s="161"/>
       <c r="O18" s="14"/>
     </row>
-    <row r="19" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" s="12"/>
-      <c r="D19" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C44</f>
+      <c r="D19" s="78" t="str">
+        <f>'Cualitativo '!C44</f>
         <v>R12</v>
       </c>
-      <c r="E19" s="160">
-        <f>'Cualitativo y Cuantitativo'!D44</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="160"/>
-      <c r="G19" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F44</f>
+      <c r="E19" s="161">
+        <f>'Cualitativo '!D44</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="161"/>
+      <c r="G19" s="80" t="str">
+        <f>'Cualitativo '!F44</f>
         <v>MUY BAJO</v>
       </c>
-      <c r="H19" s="80">
-        <f>'Cualitativo y Cuantitativo'!J44</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="80">
+      <c r="H19" s="79">
+        <f>'Cualitativo '!J44</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="79">
         <f>Matriz!K27</f>
         <v>0</v>
       </c>
-      <c r="J19" s="82"/>
-      <c r="K19" s="80"/>
-      <c r="L19" s="80">
-        <f>'Cualitativo y Cuantitativo'!J44</f>
-        <v>0</v>
-      </c>
-      <c r="M19" s="160"/>
-      <c r="N19" s="160"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="79">
+        <f>'Cualitativo '!J44</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="161"/>
+      <c r="N19" s="161"/>
       <c r="O19" s="14"/>
     </row>
-    <row r="20" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="12"/>
-      <c r="D20" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C45</f>
+      <c r="D20" s="78" t="str">
+        <f>'Cualitativo '!C45</f>
         <v>R13</v>
       </c>
-      <c r="E20" s="160">
-        <f>'Cualitativo y Cuantitativo'!D45</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="160"/>
-      <c r="G20" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F45</f>
+      <c r="E20" s="161">
+        <f>'Cualitativo '!D45</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="161"/>
+      <c r="G20" s="80" t="str">
+        <f>'Cualitativo '!F45</f>
         <v>MUY BAJO</v>
       </c>
-      <c r="H20" s="80">
-        <f>'Cualitativo y Cuantitativo'!J45</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="80">
+      <c r="H20" s="79">
+        <f>'Cualitativo '!J45</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="79">
         <f>Matriz!K28</f>
         <v>0</v>
       </c>
-      <c r="J20" s="82"/>
-      <c r="K20" s="80"/>
-      <c r="L20" s="80">
-        <f>'Cualitativo y Cuantitativo'!J45</f>
-        <v>0</v>
-      </c>
-      <c r="M20" s="160"/>
-      <c r="N20" s="160"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="79">
+        <f>'Cualitativo '!J45</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="161"/>
+      <c r="N20" s="161"/>
       <c r="O20" s="14"/>
     </row>
-    <row r="21" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="12"/>
-      <c r="D21" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C46</f>
+      <c r="D21" s="78" t="str">
+        <f>'Cualitativo '!C46</f>
         <v>R14</v>
       </c>
-      <c r="E21" s="160">
-        <f>'Cualitativo y Cuantitativo'!D46</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="160"/>
-      <c r="G21" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F46</f>
+      <c r="E21" s="161">
+        <f>'Cualitativo '!D46</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="161"/>
+      <c r="G21" s="80" t="str">
+        <f>'Cualitativo '!F46</f>
         <v>MUY BAJO</v>
       </c>
-      <c r="H21" s="80">
-        <f>'Cualitativo y Cuantitativo'!J46</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="80">
+      <c r="H21" s="79">
+        <f>'Cualitativo '!J46</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="79">
         <f>Matriz!K29</f>
         <v>0</v>
       </c>
-      <c r="J21" s="82"/>
-      <c r="K21" s="80"/>
-      <c r="L21" s="80">
-        <f>'Cualitativo y Cuantitativo'!J46</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="160"/>
-      <c r="N21" s="160"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="79">
+        <f>'Cualitativo '!J46</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="161"/>
+      <c r="N21" s="161"/>
       <c r="O21" s="14"/>
     </row>
-    <row r="22" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="12"/>
-      <c r="D22" s="79" t="str">
-        <f>'Cualitativo y Cuantitativo'!C47</f>
+      <c r="D22" s="78" t="str">
+        <f>'Cualitativo '!C47</f>
         <v>R15</v>
       </c>
-      <c r="E22" s="160">
-        <f>'Cualitativo y Cuantitativo'!D47</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="160"/>
-      <c r="G22" s="81" t="str">
-        <f>'Cualitativo y Cuantitativo'!F47</f>
+      <c r="E22" s="161">
+        <f>'Cualitativo '!D47</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="161"/>
+      <c r="G22" s="80" t="str">
+        <f>'Cualitativo '!F47</f>
         <v>MUY BAJO</v>
       </c>
-      <c r="H22" s="80">
-        <f>'Cualitativo y Cuantitativo'!J47</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="80">
+      <c r="H22" s="79">
+        <f>'Cualitativo '!J47</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="79">
         <f>Matriz!K30</f>
         <v>0</v>
       </c>
-      <c r="J22" s="82"/>
-      <c r="K22" s="80"/>
-      <c r="L22" s="80">
-        <f>'Cualitativo y Cuantitativo'!J47</f>
-        <v>0</v>
-      </c>
-      <c r="M22" s="160"/>
-      <c r="N22" s="160"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="79">
+        <f>'Cualitativo '!J47</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="161"/>
+      <c r="N22" s="161"/>
       <c r="O22" s="14"/>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
@@ -5022,7 +5048,7 @@
       <c r="N23" s="13"/>
       <c r="O23" s="14"/>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C24" s="12"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
@@ -5037,20 +5063,20 @@
       <c r="N24" s="13"/>
       <c r="O24" s="14"/>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C25" s="75"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="76"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="76"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="76"/>
-      <c r="K25" s="76"/>
-      <c r="L25" s="76"/>
-      <c r="M25" s="76"/>
-      <c r="N25" s="76"/>
-      <c r="O25" s="77"/>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C25" s="74"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="75"/>
+      <c r="L25" s="75"/>
+      <c r="M25" s="75"/>
+      <c r="N25" s="75"/>
+      <c r="O25" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="33">
@@ -5117,199 +5143,199 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="3.33203125" customWidth="1"/>
-    <col min="3" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" customWidth="1"/>
-    <col min="11" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" customWidth="1"/>
+    <col min="3" max="8" width="7.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" customWidth="1"/>
+    <col min="11" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="163" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="83">
+    <row r="5" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="164" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="82">
         <v>5</v>
       </c>
-      <c r="D5" s="104" t="str">
+      <c r="D5" s="103" t="str">
         <f>CONCATENATE(IF(AND(Matriz!H16=5,Matriz!I16=1),"R1"," "),IF(AND(Matriz!H17=5,Matriz!I17=1),"R2"," "),IF(AND(Matriz!H18=5,Matriz!I18=1),"R3"," "),IF(AND(Matriz!H19=5,Matriz!I19=1),"R4"," "),IF(AND(Matriz!H20=5,Matriz!I20=1),"R5"," "),IF(AND(Matriz!H21=5,Matriz!I21=1),"R6"," "),IF(AND(Matriz!H22=5,Matriz!I22=1)," R7"," "),IF(AND(Matriz!H23=5,Matriz!I23=1)," R8"," "),IF(AND(Matriz!H24=5,Matriz!I24=1)," R9"," "),IF(AND(Matriz!H25=5,Matriz!I25=1)," R10"," "),IF(AND(Matriz!H26=5,Matriz!I26=1)," R11"," "),IF(AND(Matriz!H27=5,Matriz!I27=1)," R12"," "),IF(AND(Matriz!H28=5,Matriz!I28=1)," R13"," "),IF(AND(Matriz!H28=5,Matriz!I28=1)," R14"," "),IF(AND(Matriz!H29=5,Matriz!I29=1)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="E5" s="104" t="str">
+      <c r="E5" s="103" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=5,Matriz!I16=2),"R1", " "), IF(AND(Matriz!H17=5,Matriz!I17=2),"R2", " "), IF(AND(Matriz!H18=5,Matriz!I18=2),"R3", " "), IF(AND(Matriz!H19=5,Matriz!I19=2),"R4", " "), IF(AND(Matriz!H20=5,Matriz!I20=2),"R5", " "), IF(AND(Matriz!H21=5,Matriz!I21=2),"R6", " "),IF(AND(Matriz!H22=5,Matriz!I22=2)," R7"," "),IF(AND(Matriz!H23=5,Matriz!I23=2)," R8"," "),IF(AND(Matriz!H24=5,Matriz!I24=2)," R9"," "),IF(AND(Matriz!H25=5,Matriz!I25=2)," R10"," "),IF(AND(Matriz!H26=5,Matriz!I26=2)," R11"," "),IF(AND(Matriz!H27=5,Matriz!I27=2)," R12"," "),IF(AND(Matriz!H28=5,Matriz!I28=2)," R13"," "),IF(AND(Matriz!H28=5,Matriz!I28=2)," R14"," "),IF(AND(Matriz!H29=5,Matriz!I29=2)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="F5" s="105" t="str">
+      <c r="F5" s="104" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=5,Matriz!I16=3),"R1", " "), IF(AND(Matriz!H17=5,Matriz!I17=3),"R2", " "), IF(AND(Matriz!H18=5,Matriz!I18=3),"R3", " "), IF(AND(Matriz!H19=52,Matriz!I19=3),"R4", " "), IF(AND(Matriz!H20=5,Matriz!I20=3),"R5", " "), IF(AND(Matriz!H21=5,Matriz!I21=3),"R6", " "),IF(AND(Matriz!H22=5,Matriz!I22=3)," R7"," "),IF(AND(Matriz!H23=5,Matriz!I23=3)," R8"," "),IF(AND(Matriz!H24=5,Matriz!I24=3)," R9"," "),IF(AND(Matriz!H25=5,Matriz!I25=3)," R10"," "),IF(AND(Matriz!H26=5,Matriz!I26=3)," R11"," "),IF(AND(Matriz!H27=5,Matriz!I27=3)," R12"," "),IF(AND(Matriz!H28=5,Matriz!I28=3)," R13"," "),IF(AND(Matriz!H28=5,Matriz!I28=3)," R14"," "),IF(AND(Matriz!H29=5,Matriz!I29=3)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="G5" s="105" t="str">
+      <c r="G5" s="104" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=5,Matriz!I16=4),"R1", " "), IF(AND(Matriz!H17=5,Matriz!I17=4),"R2", " "), IF(AND(Matriz!H18=5,Matriz!I18=4),"R3", " "), IF(AND(Matriz!H19=5,Matriz!I19=4),"R4", " "), IF(AND(Matriz!H20=5,Matriz!I20=4),"R5", " "), IF(AND(Matriz!H21=5,Matriz!I21=4),"R6", " "),IF(AND(Matriz!H22=5,Matriz!I22=4)," R7"," "),IF(AND(Matriz!H23=5,Matriz!I23=4)," R8"," "),IF(AND(Matriz!H24=5,Matriz!I24=4)," R9"," "),IF(AND(Matriz!H25=5,Matriz!I25=4)," R10"," "),IF(AND(Matriz!H26=5,Matriz!I26=4)," R11"," "),IF(AND(Matriz!H27=5,Matriz!I27=4)," R12"," "),IF(AND(Matriz!H28=5,Matriz!I28=4)," R13"," "),IF(AND(Matriz!H28=5,Matriz!I28=4)," R14"," "),IF(AND(Matriz!H29=5,Matriz!I29=4)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="H5" s="105" t="str">
+      <c r="H5" s="104" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=5,Matriz!I16=5),"R1", " "), IF(AND(Matriz!H17=5,Matriz!I17=5),"R2", " "), IF(AND(Matriz!H18=5,Matriz!I18=5),"R3", " "), IF(AND(Matriz!H19=5,Matriz!I19=5),"R4", " "), IF(AND(Matriz!H20=5,Matriz!I20=5),"R5", " "), IF(AND(Matriz!H21=5,Matriz!I21=5),"R6", " "),IF(AND(Matriz!H22=5,Matriz!I22=5)," R7"," "),IF(AND(Matriz!H23=5,Matriz!I23=5)," R8"," "),IF(AND(Matriz!H24=5,Matriz!I24=5)," R9"," "),IF(AND(Matriz!H25=5,Matriz!I25=5)," R10"," "),IF(AND(Matriz!H26=5,Matriz!I26=5)," R11"," "),IF(AND(Matriz!H27=5,Matriz!I27=5)," R12"," "),IF(AND(Matriz!H28=5,Matriz!I28=5)," R13"," "),IF(AND(Matriz!H28=5,Matriz!I28=5)," R14"," "),IF(AND(Matriz!H29=5,Matriz!I29=5)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-    </row>
-    <row r="6" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="163"/>
-      <c r="C6" s="83">
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+    </row>
+    <row r="6" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="164"/>
+      <c r="C6" s="82">
         <v>4</v>
       </c>
-      <c r="D6" s="103" t="str">
+      <c r="D6" s="102" t="str">
         <f>CONCATENATE(IF(AND(Matriz!H16=4,Matriz!I16=1),"R1"," "),IF(AND(Matriz!H17=4,Matriz!I17=1),"R2"," "),IF(AND(Matriz!H18=4,Matriz!I18=1),"R3"," "),IF(AND(Matriz!H19=4,Matriz!I19=1),"R4"," "),IF(AND(Matriz!H20=4,Matriz!I20=1),"R5"," "),IF(AND(Matriz!H21=4,Matriz!I21=1),"R6"," "),IF(AND(Matriz!H22=4,Matriz!I22=1)," R7"," "),IF(AND(Matriz!H23=4,Matriz!I23=1)," R8"," "),IF(AND(Matriz!H24=4,Matriz!I24=1)," R9"," "),IF(AND(Matriz!H25=4,Matriz!I25=1)," R10"," "),IF(AND(Matriz!H26=4,Matriz!I26=1)," R11"," "),IF(AND(Matriz!H27=4,Matriz!I27=1)," R12"," "),IF(AND(Matriz!H28=4,Matriz!I28=1)," R13"," "),IF(AND(Matriz!H28=4,Matriz!I28=1)," R14"," "),IF(AND(Matriz!H29=4,Matriz!I29=1)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="E6" s="104" t="str">
+      <c r="E6" s="103" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=4,Matriz!I16=2),"R1", " "), IF(AND(Matriz!H17=4,Matriz!I17=2),"R2", " "), IF(AND(Matriz!H18=4,Matriz!I18=2),"R3", " "), IF(AND(Matriz!H19=4,Matriz!I19=2),"R4", " "), IF(AND(Matriz!H20=4,Matriz!I20=2),"R5", " "), IF(AND(Matriz!H21=4,Matriz!I21=2),"R6", " "),IF(AND(Matriz!H22=4,Matriz!I22=2)," R7"," "),IF(AND(Matriz!H23=4,Matriz!I23=2)," R8"," "),IF(AND(Matriz!H24=4,Matriz!I24=2)," R9"," "),IF(AND(Matriz!H25=4,Matriz!I25=2)," R10"," "),IF(AND(Matriz!H26=4,Matriz!I26=2)," R11"," "),IF(AND(Matriz!H27=4,Matriz!I27=2)," R12"," "),IF(AND(Matriz!H28=4,Matriz!I28=2)," R13"," "),IF(AND(Matriz!H28=4,Matriz!I28=2)," R14"," "),IF(AND(Matriz!H29=4,Matriz!I29=2)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="F6" s="104" t="str">
+      <c r="F6" s="103" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=4,Matriz!I16=3),"R1", " "), IF(AND(Matriz!H17=4,Matriz!I17=3),"R2", " "), IF(AND(Matriz!H18=4,Matriz!I18=3),"R3", " "), IF(AND(Matriz!H19=4,Matriz!I19=3),"R4", " "), IF(AND(Matriz!H20=4,Matriz!I20=3),"R5", " "), IF(AND(Matriz!H21=4,Matriz!I21=3),"R6", " "),IF(AND(Matriz!H22=4,Matriz!I22=3)," R7"," "),IF(AND(Matriz!H23=4,Matriz!I23=3)," R8"," "),IF(AND(Matriz!H24=4,Matriz!I24=3)," R9"," "),IF(AND(Matriz!H25=4,Matriz!I25=3)," R10"," "),IF(AND(Matriz!H26=4,Matriz!I26=3)," R11"," "),IF(AND(Matriz!H27=4,Matriz!I27=3)," R12"," "),IF(AND(Matriz!H28=4,Matriz!I28=3)," R13"," "),IF(AND(Matriz!H28=4,Matriz!I28=3)," R14"," "),IF(AND(Matriz!H29=4,Matriz!I29=3)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="G6" s="105" t="str">
+      <c r="G6" s="104" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=4,Matriz!I16=4),"R1", " "), IF(AND(Matriz!H17=4,Matriz!I17=4),"R2", " "), IF(AND(Matriz!H18=4,Matriz!I18=4),"R3", " "), IF(AND(Matriz!H19=4,Matriz!I19=4),"R4", " "), IF(AND(Matriz!H20=4,Matriz!I20=4),"R5", " "), IF(AND(Matriz!H21=4,Matriz!I21=4),"R6", " "),IF(AND(Matriz!H22=4,Matriz!I22=4)," R7"," "),IF(AND(Matriz!H23=4,Matriz!I23=4)," R8"," "),IF(AND(Matriz!H24=4,Matriz!I24=4)," R9"," "),IF(AND(Matriz!H25=4,Matriz!I25=4)," R10"," "),IF(AND(Matriz!H26=4,Matriz!I26=4)," R11"," "),IF(AND(Matriz!H27=4,Matriz!I27=4)," R12"," "),IF(AND(Matriz!H28=4,Matriz!I28=4)," R13"," "),IF(AND(Matriz!H28=4,Matriz!I28=4)," R14"," "),IF(AND(Matriz!H29=4,Matriz!I29=4)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="H6" s="105" t="str">
+      <c r="H6" s="104" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=4,Matriz!I16=5),"R1", " "), IF(AND(Matriz!H17=4,Matriz!I17=5),"R2", " "), IF(AND(Matriz!H18=4,Matriz!I18=5),"R3", " "), IF(AND(Matriz!H19=4,Matriz!I19=5),"R4", " "), IF(AND(Matriz!H20=4,Matriz!I20=5),"R5", " "), IF(AND(Matriz!H21=4,Matriz!I21=5),"R6", " "),IF(AND(Matriz!H22=4,Matriz!I22=5)," R7"," "),IF(AND(Matriz!H23=4,Matriz!I23=5)," R8"," "),IF(AND(Matriz!H24=4,Matriz!I24=5)," R9"," "),IF(AND(Matriz!H25=4,Matriz!I25=5)," R10"," "),IF(AND(Matriz!H26=4,Matriz!I26=5)," R11"," "),IF(AND(Matriz!H27=4,Matriz!I27=5)," R12"," "),IF(AND(Matriz!H28=4,Matriz!I28=5)," R13"," "),IF(AND(Matriz!H28=4,Matriz!I28=5)," R14"," "),IF(AND(Matriz!H29=4,Matriz!I29=5)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-    </row>
-    <row r="7" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="163"/>
-      <c r="C7" s="83">
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="83"/>
+      <c r="M6" s="83"/>
+      <c r="N6" s="83"/>
+    </row>
+    <row r="7" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="164"/>
+      <c r="C7" s="82">
         <v>3</v>
       </c>
-      <c r="D7" s="103" t="str">
+      <c r="D7" s="102" t="str">
         <f>CONCATENATE(IF(AND(Matriz!H16=3,Matriz!I16=1),"R1"," "),IF(AND(Matriz!H17=3,Matriz!I17=1),"R2"," "),IF(AND(Matriz!H18=3,Matriz!I18=1),"R3"," "),IF(AND(Matriz!H19=3,Matriz!I19=1),"R4"," "),IF(AND(Matriz!H20=3,Matriz!I20=1),"R5"," "),IF(AND(Matriz!H21=3,Matriz!I21=1),"R6"," "),IF(AND(Matriz!H22=3,Matriz!I22=1)," R7"," "),IF(AND(Matriz!H23=3,Matriz!I23=1)," R8"," "),IF(AND(Matriz!H24=3,Matriz!I24=1)," R9"," "),IF(AND(Matriz!H25=3,Matriz!I25=1)," R10"," "),IF(AND(Matriz!H26=3,Matriz!I26=1)," R11"," "),IF(AND(Matriz!H27=3,Matriz!I27=1)," R12"," "),IF(AND(Matriz!H28=3,Matriz!I28=1)," R13"," "),IF(AND(Matriz!H28=3,Matriz!I28=1)," R14"," "),IF(AND(Matriz!H29=3,Matriz!I29=1)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="E7" s="104" t="str">
+      <c r="E7" s="103" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=3,Matriz!I16=2),"R1", " "), IF(AND(Matriz!H17=3,Matriz!I17=2),"R2", " "), IF(AND(Matriz!H18=3,Matriz!I18=2),"R3", " "), IF(AND(Matriz!H19=3,Matriz!I19=2),"R4", " "), IF(AND(Matriz!H20=3,Matriz!I20=2),"R5", " "), IF(AND(Matriz!H21=3,Matriz!I21=2),"R6", " "),IF(AND(Matriz!H22=3,Matriz!I22=2)," R7"," "),IF(AND(Matriz!H23=3,Matriz!I23=2)," R8"," "),IF(AND(Matriz!H24=3,Matriz!I24=2)," R9"," "),IF(AND(Matriz!H25=3,Matriz!I25=2)," R10"," "),IF(AND(Matriz!H26=3,Matriz!I26=2)," R11"," "),IF(AND(Matriz!H27=3,Matriz!I27=2)," R12"," "),IF(AND(Matriz!H28=3,Matriz!I28=2)," R13"," "),IF(AND(Matriz!H28=3,Matriz!I28=2)," R14"," "),IF(AND(Matriz!H29=3,Matriz!I29=2)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="F7" s="104" t="str">
+      <c r="F7" s="103" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=3,Matriz!I16=3),"R1", " "), IF(AND(Matriz!H17=3,Matriz!I17=3),"R2", " "), IF(AND(Matriz!H18=3,Matriz!I18=3),"R3", " "), IF(AND(Matriz!H19=3,Matriz!I19=3),"R4", " "), IF(AND(Matriz!H20=3,Matriz!I20=3),"R5", " "), IF(AND(Matriz!H21=3,Matriz!I21=3),"R6", " "),IF(AND(Matriz!H22=3,Matriz!I22=3)," R7"," "),IF(AND(Matriz!H23=3,Matriz!I23=3)," R8"," "),IF(AND(Matriz!H24=3,Matriz!I24=3)," R9"," "),IF(AND(Matriz!H25=3,Matriz!I25=3)," R10"," "),IF(AND(Matriz!H26=3,Matriz!I26=3)," R11"," "),IF(AND(Matriz!H27=3,Matriz!I27=3)," R12"," "),IF(AND(Matriz!H28=3,Matriz!I28=3)," R13"," "),IF(AND(Matriz!H28=3,Matriz!I28=3)," R14"," "),IF(AND(Matriz!H29=3,Matriz!I29=3)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="G7" s="104" t="str">
+      <c r="G7" s="103" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=3,Matriz!I16=4),"R1", " "), IF(AND(Matriz!H17=3,Matriz!I17=4),"R2", " "), IF(AND(Matriz!H18=3,Matriz!I18=4),"R3", " "), IF(AND(Matriz!H19=3,Matriz!I19=4),"R4", " "), IF(AND(Matriz!H20=3,Matriz!I20=4),"R5", " "), IF(AND(Matriz!H21=3,Matriz!I21=4),"R6", " "),IF(AND(Matriz!H22=3,Matriz!I22=4)," R7"," "),IF(AND(Matriz!H23=3,Matriz!I23=4)," R8"," "),IF(AND(Matriz!H24=3,Matriz!I24=4)," R9"," "),IF(AND(Matriz!H25=3,Matriz!I25=4)," R10"," "),IF(AND(Matriz!H26=3,Matriz!I26=4)," R11"," "),IF(AND(Matriz!H27=3,Matriz!I27=4)," R12"," "),IF(AND(Matriz!H28=3,Matriz!I28=4)," R13"," "),IF(AND(Matriz!H28=3,Matriz!I28=4)," R14"," "),IF(AND(Matriz!H29=3,Matriz!I29=4)," R15"," "))</f>
-        <v xml:space="preserve">R1R2R3 R5          </v>
-      </c>
-      <c r="H7" s="105" t="str">
+        <v xml:space="preserve"> R2R3 R5          </v>
+      </c>
+      <c r="H7" s="104" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=3,Matriz!I16=5),"R1", " "), IF(AND(Matriz!H17=3,Matriz!I17=5),"R2", " "), IF(AND(Matriz!H18=3,Matriz!I18=5),"R3", " "), IF(AND(Matriz!H19=3,Matriz!I19=5),"R4", " "), IF(AND(Matriz!H20=3,Matriz!I20=5),"R5", " "), IF(AND(Matriz!H21=3,Matriz!I21=5),"R6", " "),IF(AND(Matriz!H22=3,Matriz!I22=5)," R7"," "),IF(AND(Matriz!H23=3,Matriz!I23=5)," R8"," "),IF(AND(Matriz!H24=3,Matriz!I24=5)," R9"," "),IF(AND(Matriz!H25=3,Matriz!I25=5)," R10"," "),IF(AND(Matriz!H26=3,Matriz!I26=5)," R11"," "),IF(AND(Matriz!H27=3,Matriz!I27=5)," R12"," "),IF(AND(Matriz!H28=3,Matriz!I28=5)," R13"," "),IF(AND(Matriz!H28=3,Matriz!I28=5)," R14"," "),IF(AND(Matriz!H29=3,Matriz!I29=5)," R15"," "))</f>
-        <v xml:space="preserve">     R6         </v>
-      </c>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="84"/>
-      <c r="M7" s="84"/>
-      <c r="N7" s="84"/>
-    </row>
-    <row r="8" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="163"/>
-      <c r="C8" s="83">
+        <v xml:space="preserve">R1    R6         </v>
+      </c>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="83"/>
+    </row>
+    <row r="8" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="164"/>
+      <c r="C8" s="82">
         <v>2</v>
       </c>
-      <c r="D8" s="103" t="str">
+      <c r="D8" s="102" t="str">
         <f>CONCATENATE(IF(AND(Matriz!H16=2,Matriz!I16=1),"R1"," "),IF(AND(Matriz!H17=2,Matriz!I17=1),"R2"," "),IF(AND(Matriz!H18=2,Matriz!I18=1),"R3"," "),IF(AND(Matriz!H19=2,Matriz!I19=1),"R4"," "),IF(AND(Matriz!H20=2,Matriz!I20=1),"R5"," "),IF(AND(Matriz!H21=2,Matriz!I21=1),"R6"," "),IF(AND(Matriz!H22=2,Matriz!I22=1)," R7"," "),IF(AND(Matriz!H23=2,Matriz!I23=1)," R8"," "),IF(AND(Matriz!H24=2,Matriz!I24=1)," R9"," "),IF(AND(Matriz!H25=2,Matriz!I25=1)," R10"," "),IF(AND(Matriz!H26=2,Matriz!I26=1)," R11"," "),IF(AND(Matriz!H27=2,Matriz!I27=1)," R12"," "),IF(AND(Matriz!H28=2,Matriz!I28=1)," R13"," "),IF(AND(Matriz!H28=2,Matriz!I28=1)," R14"," "),IF(AND(Matriz!H29=2,Matriz!I29=1)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="E8" s="103" t="str">
+      <c r="E8" s="102" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=2,Matriz!I16=2),"R1", " "), IF(AND(Matriz!H17=2,Matriz!I17=2),"R2", " "), IF(AND(Matriz!H18=2,Matriz!I18=2),"R3", " "), IF(AND(Matriz!H19=2,Matriz!I19=2),"R4", " "), IF(AND(Matriz!H20=2,Matriz!I20=2),"R5", " "), IF(AND(Matriz!H21=2,Matriz!I21=2),"R6", " "),IF(AND(Matriz!H22=2,Matriz!I22=2)," R7"," "),IF(AND(Matriz!H23=2,Matriz!I23=2)," R8"," "),IF(AND(Matriz!H24=2,Matriz!I24=2)," R9"," "),IF(AND(Matriz!H25=2,Matriz!I25=2)," R10"," "),IF(AND(Matriz!H26=2,Matriz!I26=2)," R11"," "),IF(AND(Matriz!H27=2,Matriz!I27=2)," R12"," "),IF(AND(Matriz!H28=2,Matriz!I28=2)," R13"," "),IF(AND(Matriz!H28=2,Matriz!I28=2)," R14"," "),IF(AND(Matriz!H29=2,Matriz!I29=2)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="F8" s="104" t="str">
+      <c r="F8" s="103" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=2,Matriz!I16=3),"R1", " "), IF(AND(Matriz!H17=2,Matriz!I17=3),"R2", " "), IF(AND(Matriz!H18=2,Matriz!I18=3),"R3", " "), IF(AND(Matriz!H19=2,Matriz!I19=3),"R4", " "), IF(AND(Matriz!H20=2,Matriz!I20=3),"R5", " "), IF(AND(Matriz!H21=2,Matriz!I21=3),"R6", " "),IF(AND(Matriz!H22=2,Matriz!I22=3)," R7"," "),IF(AND(Matriz!H23=2,Matriz!I23=3)," R8"," "),IF(AND(Matriz!H24=2,Matriz!I24=3)," R9"," "),IF(AND(Matriz!H25=2,Matriz!I25=3)," R10"," "),IF(AND(Matriz!H26=2,Matriz!I26=3)," R11"," "),IF(AND(Matriz!H27=2,Matriz!I27=3)," R12"," "),IF(AND(Matriz!H28=2,Matriz!I28=3)," R13"," "),IF(AND(Matriz!H28=2,Matriz!I28=3)," R14"," "),IF(AND(Matriz!H29=2,Matriz!I29=3)," R15"," "))</f>
         <v xml:space="preserve">   R4           </v>
       </c>
-      <c r="G8" s="104" t="str">
+      <c r="G8" s="103" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=2,Matriz!I16=4),"R1", " "), IF(AND(Matriz!H17=2,Matriz!I17=4),"R2", " "), IF(AND(Matriz!H18=2,Matriz!I18=4),"R3", " "), IF(AND(Matriz!H19=2,Matriz!I19=4),"R4", " "), IF(AND(Matriz!H20=2,Matriz!I20=4),"R5", " "), IF(AND(Matriz!H21=2,Matriz!I21=4),"R6", " "),IF(AND(Matriz!H22=2,Matriz!I22=4)," R7"," "),IF(AND(Matriz!H23=2,Matriz!I23=4)," R8"," "),IF(AND(Matriz!H24=2,Matriz!I24=4)," R9"," "),IF(AND(Matriz!H25=2,Matriz!I25=4)," R10"," "),IF(AND(Matriz!H26=2,Matriz!I26=4)," R11"," "),IF(AND(Matriz!H27=2,Matriz!I27=4)," R12"," "),IF(AND(Matriz!H28=2,Matriz!I28=4)," R13"," "),IF(AND(Matriz!H28=2,Matriz!I28=4)," R14"," "),IF(AND(Matriz!H29=2,Matriz!I29=4)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="H8" s="105" t="str">
+      <c r="H8" s="104" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=2,Matriz!I16=5),"R1", " "), IF(AND(Matriz!H17=2,Matriz!I17=5),"R2", " "), IF(AND(Matriz!H18=2,Matriz!I18=5),"R3", " "), IF(AND(Matriz!H19=2,Matriz!I19=5),"R4", " "), IF(AND(Matriz!H20=2,Matriz!I20=5),"R5", " "), IF(AND(Matriz!H21=2,Matriz!I21=5),"R6", " "),IF(AND(Matriz!H22=2,Matriz!I22=5)," R7"," "),IF(AND(Matriz!H23=2,Matriz!I23=5)," R8"," "),IF(AND(Matriz!H24=2,Matriz!I24=5)," R9"," "),IF(AND(Matriz!H25=2,Matriz!I25=5)," R10"," "),IF(AND(Matriz!H26=2,Matriz!I26=5)," R11"," "),IF(AND(Matriz!H27=2,Matriz!I27=5)," R12"," "),IF(AND(Matriz!H28=2,Matriz!I28=5)," R13"," "),IF(AND(Matriz!H28=2,Matriz!I28=5)," R14"," "),IF(AND(Matriz!H29=2,Matriz!I29=5)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="84"/>
-      <c r="M8" s="84"/>
-      <c r="N8" s="84"/>
-    </row>
-    <row r="9" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="163"/>
-      <c r="C9" s="83">
+      <c r="J8" s="83"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="83"/>
+      <c r="M8" s="83"/>
+      <c r="N8" s="83"/>
+    </row>
+    <row r="9" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="164"/>
+      <c r="C9" s="82">
         <v>1</v>
       </c>
-      <c r="D9" s="103" t="str">
+      <c r="D9" s="102" t="str">
         <f>CONCATENATE(IF(AND(Matriz!H16=1,Matriz!I16=1),"R1"," "),IF(AND(Matriz!H17=1,Matriz!I17=1),"R2"," "),IF(AND(Matriz!H18=1,Matriz!I18=1),"R3"," "),IF(AND(Matriz!H19=1,Matriz!I19=1),"R4"," "),IF(AND(Matriz!H20=1,Matriz!I20=1),"R5"," "),IF(AND(Matriz!H21=1,Matriz!I21=1),"R6"," "),IF(AND(Matriz!H22=1,Matriz!I22=1)," R7"," "),IF(AND(Matriz!H23=1,Matriz!I23=1)," R8"," "),IF(AND(Matriz!H24=1,Matriz!I24=1)," R9"," "),IF(AND(Matriz!H25=1,Matriz!I25=1)," R10"," "),IF(AND(Matriz!H26=1,Matriz!I26=1)," R11"," "),IF(AND(Matriz!H27=1,Matriz!I27=1)," R12"," "),IF(AND(Matriz!H28=1,Matriz!I28=1)," R13"," "),IF(AND(Matriz!H28=1,Matriz!I28=1)," R14"," "),IF(AND(Matriz!H29=1,Matriz!I29=1)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="E9" s="103" t="str">
+      <c r="E9" s="102" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=1,Matriz!I16=2),"R1", " "), IF(AND(Matriz!H17=1,Matriz!I17=2),"R2", " "), IF(AND(Matriz!H18=1,Matriz!I18=2),"R3", " "), IF(AND(Matriz!H19=1,Matriz!I19=2),"R4", " "), IF(AND(Matriz!H20=1,Matriz!I20=2),"R5", " "), IF(AND(Matriz!H21=1,Matriz!I21=2),"R6", " "),IF(AND(Matriz!H22=1,Matriz!I22=2)," R7"," "),IF(AND(Matriz!H23=1,Matriz!I23=2)," R8"," "),IF(AND(Matriz!H24=1,Matriz!I24=2)," R9"," "),IF(AND(Matriz!H25=1,Matriz!I25=2)," R10"," "),IF(AND(Matriz!H26=1,Matriz!I26=2)," R11"," "),IF(AND(Matriz!H27=1,Matriz!I27=2)," R12"," "),IF(AND(Matriz!H28=1,Matriz!I28=2)," R13"," "),IF(AND(Matriz!H28=1,Matriz!I28=2)," R14"," "),IF(AND(Matriz!H29=1,Matriz!I29=2)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="F9" s="103" t="str">
+      <c r="F9" s="102" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=1,Matriz!I16=3),"R1", " "), IF(AND(Matriz!H17=1,Matriz!I17=3),"R2", " "), IF(AND(Matriz!H18=1,Matriz!I18=3),"R3", " "), IF(AND(Matriz!H19=1,Matriz!I19=3),"R4", " "), IF(AND(Matriz!H20=1,Matriz!I20=3),"R5", " "), IF(AND(Matriz!H21=1,Matriz!I21=3),"R6", " "),IF(AND(Matriz!H22=1,Matriz!I22=3)," R7"," "),IF(AND(Matriz!H23=1,Matriz!I23=3)," R8"," "),IF(AND(Matriz!H24=1,Matriz!I24=3)," R9"," "),IF(AND(Matriz!H25=1,Matriz!I25=3)," R10"," "),IF(AND(Matriz!H26=1,Matriz!I26=3)," R11"," "),IF(AND(Matriz!H27=1,Matriz!I27=3)," R12"," "),IF(AND(Matriz!H28=1,Matriz!I28=3)," R13"," "),IF(AND(Matriz!H28=1,Matriz!I28=3)," R14"," "),IF(AND(Matriz!H29=1,Matriz!I29=3)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="G9" s="103" t="str">
+      <c r="G9" s="102" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=1,Matriz!I16=4),"R1", " "), IF(AND(Matriz!H17=1,Matriz!I17=4),"R2", " "), IF(AND(Matriz!H18=1,Matriz!I18=4),"R3", " "), IF(AND(Matriz!H19=1,Matriz!I19=4),"R4", " "), IF(AND(Matriz!H20=1,Matriz!I20=4),"R5", " "), IF(AND(Matriz!H21=1,Matriz!I21=4),"R6", " "),IF(AND(Matriz!H22=1,Matriz!I22=4)," R7"," "),IF(AND(Matriz!H23=1,Matriz!I23=4)," R8"," "),IF(AND(Matriz!H24=1,Matriz!I24=4)," R9"," "),IF(AND(Matriz!H25=1,Matriz!I25=4)," R10"," "),IF(AND(Matriz!H26=1,Matriz!I26=4)," R11"," "),IF(AND(Matriz!H27=1,Matriz!I27=4)," R12"," "),IF(AND(Matriz!H28=1,Matriz!I28=4)," R13"," "),IF(AND(Matriz!H28=1,Matriz!I28=4)," R14"," "),IF(AND(Matriz!H29=1,Matriz!I29=4)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="H9" s="103" t="str">
+      <c r="H9" s="102" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=1,Matriz!I16=5),"R1", " "), IF(AND(Matriz!H17=1,Matriz!I17=5),"R2", " "), IF(AND(Matriz!H18=1,Matriz!I18=5),"R3", " "), IF(AND(Matriz!H19=1,Matriz!I19=5),"R4", " "), IF(AND(Matriz!H20=1,Matriz!I20=5),"R5", " "), IF(AND(Matriz!H21=1,Matriz!I21=5),"R6", " "),IF(AND(Matriz!H22=1,Matriz!I22=5)," R7"," "),IF(AND(Matriz!H23=1,Matriz!I23=5)," R8"," "),IF(AND(Matriz!H24=1,Matriz!I24=5)," R9"," "),IF(AND(Matriz!H25=1,Matriz!I25=5)," R10"," "),IF(AND(Matriz!H26=1,Matriz!I26=5)," R11"," "),IF(AND(Matriz!H27=1,Matriz!I27=5)," R12"," "),IF(AND(Matriz!H28=1,Matriz!I28=5)," R13"," "),IF(AND(Matriz!H28=1,Matriz!I28=5)," R14"," "),IF(AND(Matriz!H29=1,Matriz!I29=5)," R15"," "))</f>
         <v xml:space="preserve">               </v>
       </c>
-      <c r="J9" s="84"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="84"/>
-      <c r="N9" s="84"/>
-    </row>
-    <row r="10" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="85"/>
-      <c r="D10" s="86">
+      <c r="J9" s="83"/>
+      <c r="K9" s="83"/>
+      <c r="L9" s="83"/>
+      <c r="M9" s="83"/>
+      <c r="N9" s="83"/>
+    </row>
+    <row r="10" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="84"/>
+      <c r="D10" s="85">
         <v>1</v>
       </c>
-      <c r="E10" s="86">
+      <c r="E10" s="85">
         <v>2</v>
       </c>
-      <c r="F10" s="86">
+      <c r="F10" s="85">
         <v>3</v>
       </c>
-      <c r="G10" s="86">
+      <c r="G10" s="85">
         <v>4</v>
       </c>
-      <c r="H10" s="86">
+      <c r="H10" s="85">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D11" s="164" t="s">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D11" s="165" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="164"/>
-      <c r="F11" s="164"/>
-      <c r="G11" s="164"/>
-      <c r="H11" s="164"/>
+      <c r="E11" s="165"/>
+      <c r="F11" s="165"/>
+      <c r="G11" s="165"/>
+      <c r="H11" s="165"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5333,49 +5359,49 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1025" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="165" t="s">
+    <row r="6" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D6" s="166" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="165"/>
+      <c r="E6" s="166"/>
       <c r="G6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="87" t="s">
+    <row r="7" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D7" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="87"/>
+      <c r="E7" s="86"/>
       <c r="G7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="88" t="s">
+    <row r="8" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D8" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="88"/>
+      <c r="E8" s="87"/>
       <c r="G8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="88" t="s">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D9" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="88"/>
-    </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="88" t="s">
+      <c r="E9" s="87"/>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D10" s="87" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="88"/>
+      <c r="E10" s="87"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="92Yof/q98Qz0l03Jz4uwbgDSRgW8YmfJAg3pw1EE7BIN4dg2iPxrq1GXCmtVfB1tR/nWCd0Eo2cf06hjIpQ90A==" saltValue="aWpxacXrnR+vFubBJj5Ulw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>

</xml_diff>